<commit_message>
Commit on 21 04 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="210">
   <si>
     <t>Stage</t>
   </si>
@@ -493,6 +493,165 @@
   </si>
   <si>
     <t>7131</t>
+  </si>
+  <si>
+    <t>7132</t>
+  </si>
+  <si>
+    <t>7133</t>
+  </si>
+  <si>
+    <t>7134</t>
+  </si>
+  <si>
+    <t>7135</t>
+  </si>
+  <si>
+    <t>7136</t>
+  </si>
+  <si>
+    <t>7137</t>
+  </si>
+  <si>
+    <t>7138</t>
+  </si>
+  <si>
+    <t>7140</t>
+  </si>
+  <si>
+    <t>7141</t>
+  </si>
+  <si>
+    <t>7143</t>
+  </si>
+  <si>
+    <t>7144</t>
+  </si>
+  <si>
+    <t>7145</t>
+  </si>
+  <si>
+    <t>7148</t>
+  </si>
+  <si>
+    <t>7149</t>
+  </si>
+  <si>
+    <t>7151</t>
+  </si>
+  <si>
+    <t>7152</t>
+  </si>
+  <si>
+    <t>7150</t>
+  </si>
+  <si>
+    <t>7153</t>
+  </si>
+  <si>
+    <t>7154</t>
+  </si>
+  <si>
+    <t>7155</t>
+  </si>
+  <si>
+    <t>7156</t>
+  </si>
+  <si>
+    <t>7157</t>
+  </si>
+  <si>
+    <t>7158</t>
+  </si>
+  <si>
+    <t>7159</t>
+  </si>
+  <si>
+    <t>7162</t>
+  </si>
+  <si>
+    <t>7163</t>
+  </si>
+  <si>
+    <t>7164</t>
+  </si>
+  <si>
+    <t>7165</t>
+  </si>
+  <si>
+    <t>7166</t>
+  </si>
+  <si>
+    <t>7167</t>
+  </si>
+  <si>
+    <t>7168</t>
+  </si>
+  <si>
+    <t>7169</t>
+  </si>
+  <si>
+    <t>7170</t>
+  </si>
+  <si>
+    <t>7171</t>
+  </si>
+  <si>
+    <t>7172</t>
+  </si>
+  <si>
+    <t>7173</t>
+  </si>
+  <si>
+    <t>7175</t>
+  </si>
+  <si>
+    <t>7176</t>
+  </si>
+  <si>
+    <t>7178</t>
+  </si>
+  <si>
+    <t>7179</t>
+  </si>
+  <si>
+    <t>7180</t>
+  </si>
+  <si>
+    <t>7181</t>
+  </si>
+  <si>
+    <t>7182</t>
+  </si>
+  <si>
+    <t>7185</t>
+  </si>
+  <si>
+    <t>7186</t>
+  </si>
+  <si>
+    <t>7187</t>
+  </si>
+  <si>
+    <t>7188</t>
+  </si>
+  <si>
+    <t>7189</t>
+  </si>
+  <si>
+    <t>7191</t>
+  </si>
+  <si>
+    <t>7192</t>
+  </si>
+  <si>
+    <t>7193</t>
+  </si>
+  <si>
+    <t>7194</t>
+  </si>
+  <si>
+    <t>7195</t>
   </si>
 </sst>
 </file>
@@ -2234,7 +2393,7 @@
         <v>103</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="P3" s="18" t="s">
         <v>104</v>
@@ -2290,7 +2449,7 @@
         <v>103</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>114</v>
+        <v>209</v>
       </c>
       <c r="P4" s="18" t="s">
         <v>104</v>
@@ -2338,7 +2497,7 @@
         <v>103</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="P5" s="18" t="s">
         <v>104</v>
@@ -2432,7 +2591,7 @@
         <v>103</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="P7" s="18" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
Commit on 25 o4 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="189">
   <si>
     <t>Stage</t>
   </si>
@@ -309,15 +309,27 @@
     <t>Transaction Number</t>
   </si>
   <si>
+    <t>Amend Amount</t>
+  </si>
+  <si>
+    <t>Suspend Reason</t>
+  </si>
+  <si>
     <t>Waived Charge Amount</t>
   </si>
   <si>
+    <t>Ending Date</t>
+  </si>
+  <si>
     <t>Less Exemption Date</t>
   </si>
   <si>
     <t>High Exemption Date</t>
   </si>
   <si>
+    <t>Update DataSetID</t>
+  </si>
+  <si>
     <t>TC_CW_001</t>
   </si>
   <si>
@@ -339,58 +351,88 @@
     <t xml:space="preserve">0.00 </t>
   </si>
   <si>
+    <t>01/01/2017</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
+  </si>
+  <si>
+    <t>TC_CW_003</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_003</t>
+  </si>
+  <si>
+    <t>7194</t>
+  </si>
+  <si>
+    <t>TC_CW_004</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_004</t>
+  </si>
+  <si>
+    <t>502</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>7195</t>
+  </si>
+  <si>
+    <t>TC_CW_005</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_005</t>
+  </si>
+  <si>
+    <t>7192</t>
+  </si>
+  <si>
+    <t>TC_CW_006</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_006</t>
+  </si>
+  <si>
+    <t>TC_CW_007</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_007</t>
+  </si>
+  <si>
+    <t>7193</t>
+  </si>
+  <si>
+    <t>TC_CW_019</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_019</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>9601</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Suspend</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
     <t>01/01/2018</t>
   </si>
   <si>
-    <t>01/01/2023</t>
-  </si>
-  <si>
-    <t>TC_CW_003</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_003</t>
-  </si>
-  <si>
-    <t>7114</t>
-  </si>
-  <si>
-    <t>TC_CW_004</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_004</t>
-  </si>
-  <si>
-    <t>502</t>
-  </si>
-  <si>
-    <t>034</t>
-  </si>
-  <si>
-    <t>7115</t>
-  </si>
-  <si>
-    <t>TC_CW_005</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_005</t>
-  </si>
-  <si>
-    <t>TC_CW_006</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_006</t>
-  </si>
-  <si>
-    <t>TC_CW_007</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_007</t>
-  </si>
-  <si>
-    <t>TC_CW_008</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_008</t>
+    <t>DS01_TC_CW_020</t>
+  </si>
+  <si>
+    <t>TC_CW_020</t>
   </si>
   <si>
     <t>Number Of ChequeBook</t>
@@ -468,190 +510,85 @@
     <t>CW_003</t>
   </si>
   <si>
+    <t>CW_004</t>
+  </si>
+  <si>
+    <t>CW_005</t>
+  </si>
+  <si>
+    <t>CW_006</t>
+  </si>
+  <si>
+    <t>CW_007</t>
+  </si>
+  <si>
+    <t>CW_019</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>CW_004</t>
-  </si>
-  <si>
-    <t>CW_005</t>
-  </si>
-  <si>
-    <t>CW_006</t>
-  </si>
-  <si>
-    <t>CW_007</t>
-  </si>
-  <si>
-    <t>7117</t>
-  </si>
-  <si>
-    <t>01/01/2017</t>
-  </si>
-  <si>
-    <t>7118</t>
-  </si>
-  <si>
-    <t>7131</t>
-  </si>
-  <si>
-    <t>7132</t>
-  </si>
-  <si>
-    <t>7133</t>
-  </si>
-  <si>
-    <t>7134</t>
-  </si>
-  <si>
-    <t>7135</t>
-  </si>
-  <si>
-    <t>7136</t>
-  </si>
-  <si>
-    <t>7137</t>
-  </si>
-  <si>
-    <t>7138</t>
-  </si>
-  <si>
-    <t>7140</t>
-  </si>
-  <si>
-    <t>7141</t>
-  </si>
-  <si>
-    <t>7143</t>
-  </si>
-  <si>
-    <t>7144</t>
-  </si>
-  <si>
-    <t>7145</t>
-  </si>
-  <si>
-    <t>7148</t>
-  </si>
-  <si>
-    <t>7149</t>
-  </si>
-  <si>
-    <t>7151</t>
-  </si>
-  <si>
-    <t>7152</t>
-  </si>
-  <si>
-    <t>7150</t>
-  </si>
-  <si>
-    <t>7153</t>
-  </si>
-  <si>
-    <t>7154</t>
-  </si>
-  <si>
-    <t>7155</t>
-  </si>
-  <si>
-    <t>7156</t>
-  </si>
-  <si>
-    <t>7157</t>
-  </si>
-  <si>
-    <t>7158</t>
-  </si>
-  <si>
-    <t>7159</t>
-  </si>
-  <si>
-    <t>7162</t>
-  </si>
-  <si>
-    <t>7163</t>
-  </si>
-  <si>
-    <t>7164</t>
-  </si>
-  <si>
-    <t>7165</t>
-  </si>
-  <si>
-    <t>7166</t>
-  </si>
-  <si>
-    <t>7167</t>
-  </si>
-  <si>
-    <t>7168</t>
-  </si>
-  <si>
-    <t>7169</t>
-  </si>
-  <si>
-    <t>7170</t>
-  </si>
-  <si>
-    <t>7171</t>
-  </si>
-  <si>
-    <t>7172</t>
-  </si>
-  <si>
-    <t>7173</t>
-  </si>
-  <si>
-    <t>7175</t>
-  </si>
-  <si>
-    <t>7176</t>
-  </si>
-  <si>
-    <t>7178</t>
-  </si>
-  <si>
-    <t>7179</t>
-  </si>
-  <si>
-    <t>7180</t>
-  </si>
-  <si>
-    <t>7181</t>
-  </si>
-  <si>
-    <t>7182</t>
-  </si>
-  <si>
-    <t>7185</t>
-  </si>
-  <si>
-    <t>7186</t>
-  </si>
-  <si>
-    <t>7187</t>
-  </si>
-  <si>
-    <t>7188</t>
-  </si>
-  <si>
-    <t>7189</t>
-  </si>
-  <si>
-    <t>7191</t>
-  </si>
-  <si>
-    <t>7192</t>
-  </si>
-  <si>
-    <t>7193</t>
-  </si>
-  <si>
-    <t>7194</t>
-  </si>
-  <si>
-    <t>7195</t>
+    <t>CW_020</t>
+  </si>
+  <si>
+    <t>CW_021</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_021</t>
+  </si>
+  <si>
+    <t>CW_022</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_022</t>
+  </si>
+  <si>
+    <t>CW_023</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_023</t>
+  </si>
+  <si>
+    <t>CW_024</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_024</t>
+  </si>
+  <si>
+    <t>CW_025</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_025</t>
+  </si>
+  <si>
+    <t>CW_026</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_026</t>
+  </si>
+  <si>
+    <t>7215</t>
+  </si>
+  <si>
+    <t>7216</t>
+  </si>
+  <si>
+    <t>7218</t>
+  </si>
+  <si>
+    <t>7219</t>
+  </si>
+  <si>
+    <t>7221</t>
+  </si>
+  <si>
+    <t>7222</t>
+  </si>
+  <si>
+    <t>7223</t>
+  </si>
+  <si>
+    <t>7224</t>
   </si>
 </sst>
 </file>
@@ -838,7 +775,7 @@
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -898,6 +835,14 @@
       <alignment/>
       <protection/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
@@ -919,6 +864,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -937,11 +888,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -953,57 +912,123 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="31" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="31" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1011,72 +1036,8 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="55">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
     <cellStyle name="Currency" xfId="16" builtinId="4"/>
@@ -1093,35 +1054,45 @@
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="27"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="28"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="29"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="30"/>
-    <cellStyle name="Heading_20_1" xfId="31"/>
-    <cellStyle name="Heading1_20_1" xfId="32"/>
-    <cellStyle name="Heading1_5f_20_5f_1" xfId="33"/>
-    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="34"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="35"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="36"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="37"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="38"/>
-    <cellStyle name="Heading_5f_20_5f_1" xfId="39"/>
-    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="40"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="41"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="42"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="43"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="44"/>
-    <cellStyle name="Result_20_1" xfId="45"/>
-    <cellStyle name="Result2_20_1" xfId="46"/>
-    <cellStyle name="Result2_5f_20_5f_1" xfId="47"/>
-    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="48"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="49"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="50"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="51"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="52"/>
-    <cellStyle name="Result_5f_20_5f_1" xfId="53"/>
-    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="54"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="55"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="56"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="57"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="58"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="30"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="31"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="32"/>
+    <cellStyle name="Heading_20_1" xfId="33"/>
+    <cellStyle name="Heading1_20_1" xfId="34"/>
+    <cellStyle name="Heading1_5f_20_5f_1" xfId="35"/>
+    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="36"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="37"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="38"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="39"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="40"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="41"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="42"/>
+    <cellStyle name="Heading_5f_20_5f_1" xfId="43"/>
+    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="44"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="45"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="46"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="47"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="48"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="49"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="50"/>
+    <cellStyle name="Result_20_1" xfId="51"/>
+    <cellStyle name="Result2_20_1" xfId="52"/>
+    <cellStyle name="Result2_5f_20_5f_1" xfId="53"/>
+    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="54"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="55"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="56"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="57"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="58"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="59"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="60"/>
+    <cellStyle name="Result_5f_20_5f_1" xfId="61"/>
+    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="62"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="63"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="64"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="65"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="66"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="67"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="68"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1498,21 +1469,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52921970-2ccf-4c3e-9a52-4adb97f6dab5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3eef8af2-eeea-453e-9638-3aaa1a312e09}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="31.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="37.714285714285715" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="29.714285714285715" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="25.142857142857142" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="29.571428571428573" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="34.857142857142854" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="42.142857142857146" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="33.142857142857146" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="28.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="33.0" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -1550,27 +1521,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0d456877-bdf8-4415-b68c-1c0b7a65d1ab}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fafccd3b-d20e-4a13-9c07-9139049e6f63}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="25.857142857142858" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="31.571428571428573" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="30.142857142857142" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="38.142857142857146" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="47.857142857142854" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="28.857142857142858" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="35.142857142857146" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="33.57142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="42.57142857142857" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="53.42857142857143" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -1608,25 +1579,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7f74d0c3-d4dc-4c84-8611-46a30bf80cf8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848cb0e-cc4f-4d7e-9a84-5e25cead1a71}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="46.142857142857146" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="41.0" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" style="3" width="14.571428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="51.42857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="45.714285714285715" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.05">
@@ -1652,30 +1623,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95d2f0ab-afbe-4003-b9fd-99fd66d8357d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b3154fab-3747-4cc7-9bdd-e54443a22d80}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="35.142857142857146" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="52.285714285714285" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="40.57142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="35.857142857142854" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="31.285714285714285" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="34.42857142857143" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="3" width="31.285714285714285" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="29.285714285714285" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="39.285714285714285" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="58.42857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="45.285714285714285" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="40.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="34.857142857142854" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="38.42857142857143" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="3" width="34.857142857142854" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="32.57142857142857" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.05">
@@ -1824,30 +1795,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802f7a8d-832a-4d0d-8b82-26cf88f31537}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78de3bf8-d834-4898-868c-77aa248f71f0}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="67.28571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="36.714285714285715" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="47.42857142857143" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="45.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="35.142857142857146" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="40.285714285714285" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="53.42857142857143" collapsed="true"/>
-    <col min="9" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="53.857142857142854" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="75.28571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="41.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="53.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="50.285714285714285" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="39.285714285714285" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="45.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="59.714285714285715" collapsed="true"/>
+    <col min="9" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.05">
@@ -2033,31 +2004,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3e40e0e0-f9cf-4ed4-9296-b582e8449672}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{cd1c9d9b-e02b-44bc-b4ac-7f265b08ff81}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="31.857142857142858" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="41.285714285714285" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="39.57142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="38.857142857142854" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="24.571428571428573" collapsed="true"/>
-    <col min="6" max="7" style="3" width="13.0" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="3" width="33.57142857142857" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="22.285714285714285" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="27.285714285714285" collapsed="true"/>
-    <col min="12" max="16384" style="3" width="13.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="35.42857142857143" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="46.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="44.285714285714285" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="43.285714285714285" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="27.285714285714285" collapsed="true"/>
+    <col min="6" max="7" style="3" width="14.571428571428571" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="3" width="37.42857142857143" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="24.857142857142858" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="30.428571428571427" collapsed="true"/>
+    <col min="12" max="16384" style="3" width="14.571428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -2221,41 +2192,42 @@
       <c r="J6" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ff215fcf-888c-4cce-93a1-bc12afece545}">
-  <dimension ref="A1:R8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79083a22-cc68-4971-a6a4-c3a7c7ee429d}">
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="M1">
+      <selection pane="topLeft" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.854285714285714" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="25.857142857142858" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="37.857142857142854" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="41.714285714285715" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="28.142857142857142" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="13" width="41.42857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="34.42857142857143" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="13" width="31.142857142857142" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="37.857142857142854" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="13" width="33.285714285714285" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="13" width="29.571428571428573" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="13" width="28.857142857142858" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="13" width="25.857142857142858" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="13" width="28.857142857142858" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="46.714285714285715" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="13" width="31.428571428571427" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="13" width="46.142857142857146" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="38.42857142857143" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="13" width="34.714285714285715" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="13" width="37.142857142857146" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="13" width="33.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="13" width="32.142857142857146" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="13" width="28.857142857142858" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="13" width="19.1328125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="13" width="28.285714285714285" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="13" width="20.02734375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="13" width="32.42857142857143" collapsed="true"/>
-    <col min="19" max="16384" style="13" width="12.857142857142858" collapsed="true"/>
+    <col min="16" max="18" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="13" width="22.285714285714285" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="13" width="26.142857142857142" collapsed="true"/>
+    <col min="23" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.05">
+    <row r="1" spans="1:22" ht="14.05">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -2310,16 +2282,28 @@
       <c r="R1" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="12.8">
+      <c r="S1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>63</v>
@@ -2328,13 +2312,13 @@
         <v>37</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>37</v>
@@ -2344,28 +2328,32 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O2" s="17"/>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="18"/>
+    </row>
+    <row r="3" spans="1:22" ht="12.8">
+      <c r="A3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="12.8">
-      <c r="A3" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>63</v>
@@ -2374,13 +2362,13 @@
         <v>37</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>37</v>
@@ -2390,30 +2378,34 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="12.8">
+        <v>113</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3" s="18"/>
+    </row>
+    <row r="4" spans="1:22" ht="12.8">
       <c r="A4" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>63</v>
@@ -2422,13 +2414,13 @@
         <v>37</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>37</v>
@@ -2443,33 +2435,37 @@
         <v>78</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="P4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V4" s="18"/>
+    </row>
+    <row r="5" spans="1:22" ht="12.8">
+      <c r="A5" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="Q4" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R4" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="12.8">
-      <c r="A5" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>63</v>
@@ -2478,13 +2474,13 @@
         <v>37</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>37</v>
@@ -2494,30 +2490,34 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="P5" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V5" s="18"/>
+    </row>
+    <row r="6" spans="1:22" ht="12.8">
+      <c r="A6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="12.8">
-      <c r="A6" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>63</v>
@@ -2526,13 +2526,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>37</v>
@@ -2542,28 +2542,32 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O6" s="17"/>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V6" s="18"/>
+    </row>
+    <row r="7" spans="1:22" ht="12.8">
+      <c r="A7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="12.8">
-      <c r="A7" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>63</v>
@@ -2572,13 +2576,13 @@
         <v>37</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>37</v>
@@ -2588,77 +2592,151 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="P7" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="R7" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V7" s="18"/>
+    </row>
+    <row r="8" spans="1:22" ht="12.8">
+      <c r="A8" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="12.8">
-      <c r="A8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="18" t="s">
-        <v>104</v>
+      <c r="I8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>106</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="U8" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V8" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="12.8">
+      <c r="A9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d3251586-787b-4597-963d-8aa85fe90f13}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d5491991-c04d-4c4f-b253-cd1912c1f0a0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.854285714285714" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="24.142857142857142" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="40.57142857142857" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="35.42857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="13" width="37.714285714285715" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="13" width="36.857142857142854" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="26.285714285714285" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="13" width="32.142857142857146" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="13" width="31.428571428571427" collapsed="true"/>
-    <col min="10" max="16384" style="13" width="12.857142857142858" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="13" width="26.857142857142858" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="13" width="45.285714285714285" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="39.57142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="13" width="35.142857142857146" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="13" width="42.142857142857146" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="41.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="29.285714285714285" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="13" width="35.857142857142854" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="13" width="35.0" collapsed="true"/>
+    <col min="10" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.05">
@@ -2669,39 +2747,39 @@
         <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>63</v>
@@ -2716,66 +2794,66 @@
         <v>78</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
+  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b454613e-2326-4661-a116-4f8d7079f3d9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1bcd2b3b-b633-40d0-98c8-709e49903925}">
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.574285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="21" width="12.714285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="21" width="62.285714285714285" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="21" width="47.285714285714285" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="21" width="14.142857142857142" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="21" width="69.57142857142857" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="21" width="52.857142857142854" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="21" width="14.92578125" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" style="21" width="54.57142857142857" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="21" width="36.857142857142854" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="21" width="36.42857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="21" width="35.142857142857146" collapsed="true"/>
-    <col min="11" max="16384" style="29" width="11.571428571428571" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" style="21" width="61.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="21" width="41.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="21" width="40.57142857142857" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="21" width="39.285714285714285" collapsed="true"/>
+    <col min="11" max="16384" style="29" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
       <c r="A1" s="19" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
@@ -2783,13 +2861,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
@@ -2803,13 +2881,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -2823,13 +2901,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -2843,13 +2921,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -2863,13 +2941,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -2883,13 +2961,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -2903,13 +2981,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -2919,11 +2997,21 @@
       <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="14.05">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="20"/>
+      <c r="A9" s="20">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>166</v>
+      </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -2931,10 +3019,18 @@
       <c r="J9" s="28"/>
     </row>
     <row r="10" spans="1:10" ht="14.05">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="27"/>
+      <c r="A10" s="20">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>167</v>
+      </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2943,10 +3039,18 @@
       <c r="J10" s="28"/>
     </row>
     <row r="11" spans="1:10" ht="14.05">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="27"/>
+      <c r="A11" s="20">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2955,10 +3059,18 @@
       <c r="J11" s="28"/>
     </row>
     <row r="12" spans="1:10" ht="14.05">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="27"/>
+      <c r="A12" s="20">
+        <v>11</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -2967,10 +3079,18 @@
       <c r="J12" s="28"/>
     </row>
     <row r="13" spans="1:10" ht="14.05">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="27"/>
+      <c r="A13" s="20">
+        <v>12</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -2979,10 +3099,18 @@
       <c r="J13" s="28"/>
     </row>
     <row r="14" spans="1:10" ht="14.05">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="27"/>
+      <c r="A14" s="20">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -2991,10 +3119,18 @@
       <c r="J14" s="28"/>
     </row>
     <row r="15" spans="1:10" ht="14.05">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="27"/>
+      <c r="A15" s="20">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3003,10 +3139,18 @@
       <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:10" ht="14.05">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="27"/>
+      <c r="A16" s="20">
+        <v>15</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>159</v>
+      </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>

</xml_diff>

<commit_message>
Commit on 26 04 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="CSM_Login" sheetId="1" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="190">
   <si>
     <t>Stage</t>
   </si>
@@ -315,6 +315,9 @@
     <t>Suspend Reason</t>
   </si>
   <si>
+    <t>Close Reason</t>
+  </si>
+  <si>
     <t>Waived Charge Amount</t>
   </si>
   <si>
@@ -435,6 +438,27 @@
     <t>TC_CW_020</t>
   </si>
   <si>
+    <t>TC_CW_021</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_021</t>
+  </si>
+  <si>
+    <t>TC_CW_022</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_022</t>
+  </si>
+  <si>
+    <t>Close SO</t>
+  </si>
+  <si>
+    <t>TC_CW_023</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_023</t>
+  </si>
+  <si>
     <t>Number Of ChequeBook</t>
   </si>
   <si>
@@ -525,30 +549,21 @@
     <t>CW_019</t>
   </si>
   <si>
+    <t>CW_020</t>
+  </si>
+  <si>
+    <t>CW_021</t>
+  </si>
+  <si>
+    <t>CW_022</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>CW_020</t>
-  </si>
-  <si>
-    <t>CW_021</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_021</t>
-  </si>
-  <si>
-    <t>CW_022</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_022</t>
-  </si>
-  <si>
     <t>CW_023</t>
   </si>
   <si>
-    <t>DS01_TC_CW_023</t>
-  </si>
-  <si>
     <t>CW_024</t>
   </si>
   <si>
@@ -567,28 +582,16 @@
     <t>DS01_TC_CW_026</t>
   </si>
   <si>
-    <t>7215</t>
-  </si>
-  <si>
-    <t>7216</t>
-  </si>
-  <si>
-    <t>7218</t>
-  </si>
-  <si>
-    <t>7219</t>
-  </si>
-  <si>
-    <t>7221</t>
-  </si>
-  <si>
-    <t>7222</t>
-  </si>
-  <si>
-    <t>7223</t>
-  </si>
-  <si>
-    <t>7224</t>
+    <t>7236</t>
+  </si>
+  <si>
+    <t>7237</t>
+  </si>
+  <si>
+    <t>7238</t>
+  </si>
+  <si>
+    <t>7239</t>
   </si>
 </sst>
 </file>
@@ -948,15 +951,15 @@
       <alignment/>
       <protection/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1469,7 +1472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3eef8af2-eeea-453e-9638-3aaa1a312e09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2d2fee53-bdb2-4cf9-b589-b0541c58ea4b}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1527,7 +1530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fafccd3b-d20e-4a13-9c07-9139049e6f63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72bf1212-9e52-40a2-b4a9-220f64cc8c8e}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1585,7 +1588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2848cb0e-cc4f-4d7e-9a84-5e25cead1a71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fbf29363-17cc-4990-bf68-b2070f962b39}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1629,7 +1632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b3154fab-3747-4cc7-9bdd-e54443a22d80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461a8c5d-8955-4b5e-836e-13763e63444e}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1801,7 +1804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78de3bf8-d834-4898-868c-77aa248f71f0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1b7f9738-15bf-4061-ad4b-24e77f01ed3c}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2010,7 +2013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{cd1c9d9b-e02b-44bc-b4ac-7f265b08ff81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2bf8ff76-2f39-49d8-8ca3-7e92ba03840c}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2067,10 +2070,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.05">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2097,13 +2100,13 @@
       <c r="J2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="10"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="14.05">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -2130,13 +2133,13 @@
       <c r="J3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="14.05">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -2163,33 +2166,33 @@
       <c r="J4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
@@ -2198,11 +2201,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79083a22-cc68-4971-a6a4-c3a7c7ee429d}">
-  <dimension ref="A1:V9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42356682-ae8d-425b-9846-1e008edcf923}">
+  <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="M1">
-      <selection pane="topLeft" activeCell="Q29" sqref="Q29"/>
+    <sheetView workbookViewId="0" topLeftCell="M1">
+      <selection pane="topLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="12.8"/>
@@ -2220,14 +2223,14 @@
     <col min="13" max="13" customWidth="true" style="13" width="32.142857142857146" collapsed="true"/>
     <col min="14" max="14" customWidth="true" style="13" width="28.857142857142858" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="13" width="19.1328125" collapsed="true"/>
-    <col min="16" max="18" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
-    <col min="19" max="20" customWidth="true" style="13" width="22.285714285714285" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="13" width="26.142857142857142" collapsed="true"/>
-    <col min="23" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
+    <col min="16" max="19" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" style="13" width="22.285714285714285" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="13" width="26.142857142857142" collapsed="true"/>
+    <col min="24" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.05">
+    <row r="1" spans="1:23" ht="14.05">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -2294,16 +2297,19 @@
       <c r="V1" s="16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="12.8">
+      <c r="W1" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>63</v>
@@ -2312,13 +2318,13 @@
         <v>37</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>37</v>
@@ -2328,32 +2334,33 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O2" s="17"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T2" s="15"/>
       <c r="U2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="18"/>
-    </row>
-    <row r="3" spans="1:22" ht="12.8">
+      <c r="V2" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W2" s="18"/>
+    </row>
+    <row r="3" spans="1:23" ht="12.8">
       <c r="A3" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>63</v>
@@ -2362,13 +2369,13 @@
         <v>37</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>37</v>
@@ -2378,34 +2385,35 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
-      <c r="R3" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T3" s="15"/>
       <c r="U3" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V3" s="18"/>
-    </row>
-    <row r="4" spans="1:22" ht="12.8">
+      <c r="V3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W3" s="18"/>
+    </row>
+    <row r="4" spans="1:23" ht="12.8">
       <c r="A4" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>63</v>
@@ -2414,13 +2422,13 @@
         <v>37</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>37</v>
@@ -2435,37 +2443,38 @@
         <v>78</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
-      <c r="R4" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15" t="s">
+      <c r="R4" s="15"/>
+      <c r="S4" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T4" s="15"/>
       <c r="U4" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V4" s="18"/>
-    </row>
-    <row r="5" spans="1:22" ht="12.8">
+      <c r="V4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W4" s="18"/>
+    </row>
+    <row r="5" spans="1:23" ht="12.8">
       <c r="A5" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>63</v>
@@ -2474,13 +2483,13 @@
         <v>37</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>37</v>
@@ -2490,34 +2499,35 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
-      <c r="R5" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15" t="s">
+      <c r="R5" s="15"/>
+      <c r="S5" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T5" s="15"/>
       <c r="U5" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V5" s="18"/>
-    </row>
-    <row r="6" spans="1:22" ht="12.8">
+      <c r="V5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W5" s="18"/>
+    </row>
+    <row r="6" spans="1:23" ht="12.8">
       <c r="A6" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>63</v>
@@ -2526,13 +2536,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>37</v>
@@ -2542,32 +2552,33 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
-      <c r="R6" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15" t="s">
+      <c r="R6" s="15"/>
+      <c r="S6" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T6" s="15"/>
       <c r="U6" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="1:22" ht="12.8">
+      <c r="V6" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W6" s="18"/>
+    </row>
+    <row r="7" spans="1:23" ht="12.8">
       <c r="A7" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>63</v>
@@ -2576,13 +2587,13 @@
         <v>37</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>37</v>
@@ -2592,34 +2603,35 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15" t="s">
+      <c r="R7" s="15"/>
+      <c r="S7" s="18" t="s">
         <v>109</v>
       </c>
+      <c r="T7" s="15"/>
       <c r="U7" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V7" s="18"/>
-    </row>
-    <row r="8" spans="1:22" ht="12.8">
+      <c r="V7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W7" s="18"/>
+    </row>
+    <row r="8" spans="1:23" ht="12.8">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>63</v>
@@ -2628,13 +2640,13 @@
         <v>37</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>37</v>
@@ -2643,7 +2655,7 @@
         <v>63</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>39</v>
@@ -2652,39 +2664,38 @@
         <v>66</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>188</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="O8" s="17"/>
       <c r="P8" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="R8" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S8" s="15" t="s">
         <v>133</v>
+      </c>
+      <c r="R8" s="15"/>
+      <c r="S8" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="T8" s="15" t="s">
         <v>134</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="V8" s="18" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="12.8">
+      <c r="V8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W8" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="12.8">
       <c r="A9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -2698,18 +2709,210 @@
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
-      <c r="O9" s="17" t="s">
-        <v>188</v>
-      </c>
+      <c r="O9" s="17"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
-      <c r="R9" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="S9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
-      <c r="V9" s="18"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" ht="12.8">
+      <c r="A10" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" spans="1:23" ht="12.8">
+      <c r="A11" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="V11" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W11" s="18"/>
+    </row>
+    <row r="12" spans="1:23" ht="12.8">
+      <c r="A12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="O12" s="17"/>
+      <c r="P12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="T12" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="W12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
@@ -2718,7 +2921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d5491991-c04d-4c4f-b253-cd1912c1f0a0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8943832f-6cab-4da4-801c-f7f484f9d0c8}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2747,39 +2950,39 @@
         <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>63</v>
@@ -2794,7 +2997,7 @@
         <v>78</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2804,11 +3007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1bcd2b3b-b633-40d0-98c8-709e49903925}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4dd1afa3-5f7e-46a3-a008-ae51cbf7edcf}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A6">
+      <selection pane="topLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
@@ -2816,7 +3019,7 @@
     <col min="1" max="1" customWidth="true" style="21" width="14.142857142857142" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="21" width="69.57142857142857" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="21" width="52.857142857142854" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="21" width="14.92578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="21" width="16.571428571428573" collapsed="true"/>
     <col min="5" max="7" customWidth="true" style="21" width="61.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="21" width="41.0" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="21" width="40.57142857142857" collapsed="true"/>
@@ -2826,34 +3029,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
       <c r="A1" s="19" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
@@ -2861,13 +3064,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
@@ -2881,13 +3084,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -2901,13 +3104,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -2921,13 +3124,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -2941,13 +3144,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -2961,13 +3164,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -2981,13 +3184,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -3001,16 +3204,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -3023,10 +3226,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>167</v>
@@ -3043,13 +3246,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -3063,13 +3266,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -3083,13 +3286,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
@@ -3103,13 +3306,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -3123,13 +3326,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -3143,13 +3346,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>

</xml_diff>

<commit_message>
Commit on 27 Apr 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="192">
   <si>
     <t>Stage</t>
   </si>
@@ -318,6 +318,9 @@
     <t>Close Reason</t>
   </si>
   <si>
+    <t>Cancel Reason</t>
+  </si>
+  <si>
     <t>Waived Charge Amount</t>
   </si>
   <si>
@@ -459,6 +462,9 @@
     <t>DS01_TC_CW_023</t>
   </si>
   <si>
+    <t>CANCEL TRX</t>
+  </si>
+  <si>
     <t>Number Of ChequeBook</t>
   </si>
   <si>
@@ -558,40 +564,40 @@
     <t>CW_022</t>
   </si>
   <si>
+    <t>CW_023</t>
+  </si>
+  <si>
+    <t>CW_024</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_024</t>
+  </si>
+  <si>
+    <t>CW_025</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_025</t>
+  </si>
+  <si>
+    <t>CW_026</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_026</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>CW_023</t>
-  </si>
-  <si>
-    <t>CW_024</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_024</t>
-  </si>
-  <si>
-    <t>CW_025</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_025</t>
-  </si>
-  <si>
-    <t>CW_026</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_026</t>
-  </si>
-  <si>
-    <t>7236</t>
-  </si>
-  <si>
-    <t>7237</t>
-  </si>
-  <si>
-    <t>7238</t>
-  </si>
-  <si>
-    <t>7239</t>
+    <t>7241</t>
+  </si>
+  <si>
+    <t>7242</t>
+  </si>
+  <si>
+    <t>7244</t>
+  </si>
+  <si>
+    <t>7250</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2d2fee53-bdb2-4cf9-b589-b0541c58ea4b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6fe5b943-4056-4df0-b65e-a2cbbfe4b120}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1530,7 +1536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72bf1212-9e52-40a2-b4a9-220f64cc8c8e}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33c41bce-3be9-4971-8f4a-e87afdc57aca}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1588,7 +1594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fbf29363-17cc-4990-bf68-b2070f962b39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{bf44031a-a65d-4d1a-bb23-dbab3b22da6d}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1632,7 +1638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461a8c5d-8955-4b5e-836e-13763e63444e}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96db8615-4bb0-4c9a-8d94-7f6c787d4f01}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -1804,7 +1810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1b7f9738-15bf-4061-ad4b-24e77f01ed3c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ff3322e-4881-42c7-8c19-65e2fe074983}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2013,7 +2019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2bf8ff76-2f39-49d8-8ca3-7e92ba03840c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89339952-aacb-493b-beb3-bcc837169278}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2201,11 +2207,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42356682-ae8d-425b-9846-1e008edcf923}">
-  <dimension ref="A1:W12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91bd02d4-0f5c-42f5-9848-e4177bcf4886}">
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="M1">
-      <selection pane="topLeft" activeCell="Q19" sqref="Q19"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="12.8"/>
@@ -2223,14 +2229,14 @@
     <col min="13" max="13" customWidth="true" style="13" width="32.142857142857146" collapsed="true"/>
     <col min="14" max="14" customWidth="true" style="13" width="28.857142857142858" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="13" width="19.1328125" collapsed="true"/>
-    <col min="16" max="19" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
-    <col min="20" max="21" customWidth="true" style="13" width="22.285714285714285" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="13" width="26.142857142857142" collapsed="true"/>
-    <col min="24" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
+    <col min="16" max="20" customWidth="true" style="13" width="31.571428571428573" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" style="13" width="22.285714285714285" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="13" width="26.142857142857142" collapsed="true"/>
+    <col min="25" max="16384" style="13" width="14.428571428571429" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.05">
+    <row r="1" spans="1:24" ht="14.05">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -2300,16 +2306,19 @@
       <c r="W1" s="16" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="12.8">
+      <c r="X1" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>63</v>
@@ -2318,13 +2327,13 @@
         <v>37</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>37</v>
@@ -2334,33 +2343,34 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O2" s="17"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U2" s="15"/>
       <c r="V2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="18"/>
-    </row>
-    <row r="3" spans="1:23" ht="12.8">
+      <c r="W2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X2" s="18"/>
+    </row>
+    <row r="3" spans="1:24" ht="12.8">
       <c r="A3" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>63</v>
@@ -2369,13 +2379,13 @@
         <v>37</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>37</v>
@@ -2385,35 +2395,36 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
-      <c r="S3" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15" t="s">
+      <c r="S3" s="15"/>
+      <c r="T3" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U3" s="15"/>
       <c r="V3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W3" s="18"/>
-    </row>
-    <row r="4" spans="1:23" ht="12.8">
+      <c r="W3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X3" s="18"/>
+    </row>
+    <row r="4" spans="1:24" ht="12.8">
       <c r="A4" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>63</v>
@@ -2422,13 +2433,13 @@
         <v>37</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>37</v>
@@ -2443,38 +2454,39 @@
         <v>78</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
-      <c r="S4" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15" t="s">
+      <c r="S4" s="15"/>
+      <c r="T4" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U4" s="15"/>
       <c r="V4" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W4" s="18"/>
-    </row>
-    <row r="5" spans="1:23" ht="12.8">
+      <c r="W4" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X4" s="18"/>
+    </row>
+    <row r="5" spans="1:24" ht="12.8">
       <c r="A5" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>63</v>
@@ -2483,13 +2495,13 @@
         <v>37</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>37</v>
@@ -2499,35 +2511,36 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
-      <c r="S5" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15" t="s">
+      <c r="S5" s="15"/>
+      <c r="T5" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U5" s="15"/>
       <c r="V5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W5" s="18"/>
-    </row>
-    <row r="6" spans="1:23" ht="12.8">
+      <c r="W5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X5" s="18"/>
+    </row>
+    <row r="6" spans="1:24" ht="12.8">
       <c r="A6" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>63</v>
@@ -2536,13 +2549,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>37</v>
@@ -2552,33 +2565,34 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15" t="s">
+      <c r="S6" s="15"/>
+      <c r="T6" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U6" s="15"/>
       <c r="V6" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W6" s="18"/>
-    </row>
-    <row r="7" spans="1:23" ht="12.8">
+      <c r="W6" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X6" s="18"/>
+    </row>
+    <row r="7" spans="1:24" ht="12.8">
       <c r="A7" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>63</v>
@@ -2587,13 +2601,13 @@
         <v>37</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>37</v>
@@ -2603,35 +2617,36 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
-      <c r="S7" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15" t="s">
+      <c r="S7" s="15"/>
+      <c r="T7" s="18" t="s">
         <v>110</v>
       </c>
+      <c r="U7" s="15"/>
       <c r="V7" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="W7" s="18"/>
-    </row>
-    <row r="8" spans="1:23" ht="12.8">
+      <c r="W7" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X7" s="18"/>
+    </row>
+    <row r="8" spans="1:24" ht="12.8">
       <c r="A8" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>63</v>
@@ -2640,13 +2655,13 @@
         <v>37</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>37</v>
@@ -2655,7 +2670,7 @@
         <v>63</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>39</v>
@@ -2664,38 +2679,39 @@
         <v>66</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O8" s="17"/>
       <c r="P8" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R8" s="15"/>
-      <c r="S8" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T8" s="15" t="s">
-        <v>134</v>
+      <c r="S8" s="15"/>
+      <c r="T8" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="U8" s="15" t="s">
         <v>135</v>
       </c>
       <c r="V8" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="W8" s="18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="12.8">
+      <c r="W8" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X8" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="12.8">
       <c r="A9" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -2713,23 +2729,24 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
-      <c r="S9" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="U9" s="15"/>
       <c r="V9" s="15"/>
-      <c r="W9" s="18"/>
-    </row>
-    <row r="10" spans="1:23" ht="12.8">
+      <c r="W9" s="15"/>
+      <c r="X9" s="18"/>
+    </row>
+    <row r="10" spans="1:24" ht="12.8">
       <c r="A10" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>63</v>
@@ -2738,13 +2755,13 @@
         <v>37</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>37</v>
@@ -2753,7 +2770,7 @@
         <v>63</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>39</v>
@@ -2762,37 +2779,38 @@
         <v>66</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
-      <c r="S10" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T10" s="15" t="s">
-        <v>134</v>
+      <c r="S10" s="15"/>
+      <c r="T10" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="U10" s="15" t="s">
         <v>135</v>
       </c>
       <c r="V10" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="W10" s="18"/>
-    </row>
-    <row r="11" spans="1:23" ht="12.8">
+        <v>136</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X10" s="18"/>
+    </row>
+    <row r="11" spans="1:24" ht="12.8">
       <c r="A11" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>63</v>
@@ -2801,13 +2819,13 @@
         <v>37</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>37</v>
@@ -2816,7 +2834,7 @@
         <v>63</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>39</v>
@@ -2825,41 +2843,40 @@
         <v>66</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="O11" s="17" t="s">
-        <v>189</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="O11" s="17"/>
       <c r="P11" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q11" s="15"/>
       <c r="R11" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="S11" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T11" s="15" t="s">
-        <v>134</v>
+        <v>143</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="U11" s="15" t="s">
         <v>135</v>
       </c>
       <c r="V11" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="W11" s="18"/>
-    </row>
-    <row r="12" spans="1:23" ht="12.8">
+        <v>136</v>
+      </c>
+      <c r="W11" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X11" s="18"/>
+    </row>
+    <row r="12" spans="1:24" ht="12.8">
       <c r="A12" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>63</v>
@@ -2868,13 +2885,13 @@
         <v>37</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>37</v>
@@ -2883,7 +2900,7 @@
         <v>63</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>39</v>
@@ -2892,27 +2909,32 @@
         <v>66</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="O12" s="17"/>
+        <v>109</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="P12" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
-      <c r="S12" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="T12" s="15" t="s">
-        <v>134</v>
+      <c r="S12" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="T12" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="U12" s="15" t="s">
         <v>135</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="W12" s="18"/>
+        <v>136</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="X12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
@@ -2921,7 +2943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8943832f-6cab-4da4-801c-f7f484f9d0c8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91e4a0db-6c12-4ae1-bd6b-b58725577cce}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
@@ -2950,39 +2972,39 @@
         <v>11</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>63</v>
@@ -2997,7 +3019,7 @@
         <v>78</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3007,11 +3029,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4dd1afa3-5f7e-46a3-a008-ae51cbf7edcf}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1c031869-08b1-4bd7-bad9-9b91f830ca74}">
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A6">
-      <selection pane="topLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.004285714285713" defaultRowHeight="14.05"/>
@@ -3019,7 +3041,7 @@
     <col min="1" max="1" customWidth="true" style="21" width="14.142857142857142" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="21" width="69.57142857142857" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="21" width="52.857142857142854" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="21" width="16.571428571428573" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="21" width="14.92578125" collapsed="true"/>
     <col min="5" max="7" customWidth="true" style="21" width="61.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="21" width="41.0" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="21" width="40.57142857142857" collapsed="true"/>
@@ -3029,34 +3051,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
       <c r="A1" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
@@ -3064,13 +3086,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
@@ -3084,13 +3106,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -3104,13 +3126,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>169</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>167</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -3124,13 +3146,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
@@ -3144,13 +3166,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -3164,13 +3186,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -3184,13 +3206,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
@@ -3204,16 +3226,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -3226,13 +3248,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -3246,13 +3268,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -3266,13 +3288,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -3286,13 +3308,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
@@ -3306,13 +3328,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -3326,13 +3348,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -3346,13 +3368,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>

</xml_diff>

<commit_message>
Commit on 9 may 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CSM_Login" sheetId="1" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="256">
   <si>
     <t>Stage</t>
   </si>
@@ -374,7 +374,7 @@
     <t>DS01_TC_CW_003</t>
   </si>
   <si>
-    <t>7277</t>
+    <t>7291</t>
   </si>
   <si>
     <t>TC_CW_004</t>
@@ -389,7 +389,7 @@
     <t>034</t>
   </si>
   <si>
-    <t>7278</t>
+    <t>7292</t>
   </si>
   <si>
     <t>TC_CW_005</t>
@@ -398,7 +398,7 @@
     <t>DS01_TC_CW_005</t>
   </si>
   <si>
-    <t>7279</t>
+    <t>7293</t>
   </si>
   <si>
     <t>TC_CW_006</t>
@@ -407,270 +407,374 @@
     <t>DS01_TC_CW_006</t>
   </si>
   <si>
+    <t>7294</t>
+  </si>
+  <si>
     <t>TC_CW_007</t>
   </si>
   <si>
     <t>DS01_TC_CW_007</t>
   </si>
   <si>
+    <t>7295</t>
+  </si>
+  <si>
+    <t>TC_CW_019</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_019</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>9601</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Suspend</t>
+  </si>
+  <si>
+    <t>01/01/2021</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_020</t>
+  </si>
+  <si>
+    <t>TC_CW_020</t>
+  </si>
+  <si>
+    <t>TC_CW_021</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_021</t>
+  </si>
+  <si>
+    <t>TC_CW_022</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_022</t>
+  </si>
+  <si>
+    <t>Close SO</t>
+  </si>
+  <si>
+    <t>TC_CW_023</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_023</t>
+  </si>
+  <si>
+    <t>7250</t>
+  </si>
+  <si>
+    <t>CANCEL TRX</t>
+  </si>
+  <si>
+    <t>Request Number</t>
+  </si>
+  <si>
+    <t>Reason on rejection</t>
+  </si>
+  <si>
+    <t>Number Of ChequeBook</t>
+  </si>
+  <si>
+    <t>Cheque Code</t>
+  </si>
+  <si>
+    <t>account Branch Code</t>
+  </si>
+  <si>
+    <t>Account Currency Code</t>
+  </si>
+  <si>
+    <t>Account Gl code</t>
+  </si>
+  <si>
+    <t>Account CIF Code</t>
+  </si>
+  <si>
+    <t>Account Serial Number</t>
+  </si>
+  <si>
+    <t>ChequeBook Request Number</t>
+  </si>
+  <si>
+    <t>ChequeFrom Number</t>
+  </si>
+  <si>
+    <t>ChequeFrom To Number</t>
+  </si>
+  <si>
+    <t>TC_CW_002</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_002</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>CHB_081</t>
+  </si>
+  <si>
+    <t>DS01_TC_CHB_081</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>96123</t>
+  </si>
+  <si>
+    <t>CHB_123_124_Prereq_01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DS01_TC_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>CHB_123_124_Prereq</t>
+    </r>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>CHB_123_124_Prereq_02</t>
+  </si>
+  <si>
+    <t>CHB_123</t>
+  </si>
+  <si>
+    <t>DS01_TC_CHB_123</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>CHB_124</t>
+  </si>
+  <si>
+    <t>DS01_TC_CHB_124</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>Data Set ID</t>
+  </si>
+  <si>
+    <t>ExecuteYes/No</t>
+  </si>
+  <si>
+    <t>Dependent Test Case Id_One</t>
+  </si>
+  <si>
+    <t>Dependent Test Case Id_Two</t>
+  </si>
+  <si>
+    <t>Dependent Test Case Id_Three</t>
+  </si>
+  <si>
+    <t>Dependent Test Case Id_Four</t>
+  </si>
+  <si>
+    <t>Dependent Test Case Id_Five</t>
+  </si>
+  <si>
+    <t>Dependent Data Set Id_Five</t>
+  </si>
+  <si>
+    <t>CW_001</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>CW_002</t>
+  </si>
+  <si>
+    <t>CW_003</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>CW_004</t>
+  </si>
+  <si>
+    <t>CW_005</t>
+  </si>
+  <si>
+    <t>CW_006</t>
+  </si>
+  <si>
+    <t>CW_007</t>
+  </si>
+  <si>
+    <t>CW_019</t>
+  </si>
+  <si>
+    <t>CW_020</t>
+  </si>
+  <si>
+    <t>CW_021</t>
+  </si>
+  <si>
+    <t>CW_022</t>
+  </si>
+  <si>
+    <t>CW_023</t>
+  </si>
+  <si>
+    <t>CW_024</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_024</t>
+  </si>
+  <si>
+    <t>CW_025</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_025</t>
+  </si>
+  <si>
+    <t>CW_026</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_026</t>
+  </si>
+  <si>
+    <t>CW_038</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_038</t>
+  </si>
+  <si>
+    <t>CW_039</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_039</t>
+  </si>
+  <si>
+    <t>CW_040</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_040</t>
+  </si>
+  <si>
+    <t>CW_041</t>
+  </si>
+  <si>
+    <t>DS01_TC_CW_041</t>
+  </si>
+  <si>
+    <t>CHB_112</t>
+  </si>
+  <si>
+    <t>CHB_113</t>
+  </si>
+  <si>
+    <t>CHB_119</t>
+  </si>
+  <si>
+    <t>CHB_120</t>
+  </si>
+  <si>
+    <t>CHB_121</t>
+  </si>
+  <si>
+    <t>ChequeBookPrerequisites_01</t>
+  </si>
+  <si>
+    <t>CHB_123_124_Prereq</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DS01_TC_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>CHB_123_124_Prereq</t>
+    </r>
+  </si>
+  <si>
+    <t>CHB_122</t>
+  </si>
+  <si>
+    <t>ChequeBookPrerequisites_02</t>
+  </si>
+  <si>
+    <t>ChequeBookPrerequisites_03</t>
+  </si>
+  <si>
+    <t>Certificate Type</t>
+  </si>
+  <si>
+    <t>CIF Number</t>
+  </si>
+  <si>
+    <t>Number Of Bills</t>
+  </si>
+  <si>
+    <t>Total Amount Of Bills</t>
+  </si>
+  <si>
+    <t>Passbook Code</t>
+  </si>
+  <si>
+    <t>Passbook Type</t>
+  </si>
+  <si>
+    <t>01/01/2017</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
+  </si>
+  <si>
+    <t>7194</t>
+  </si>
+  <si>
+    <t>7195</t>
+  </si>
+  <si>
+    <t>7192</t>
+  </si>
+  <si>
     <t>7193</t>
   </si>
   <si>
-    <t>TC_CW_019</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_019</t>
-  </si>
-  <si>
-    <t>326</t>
-  </si>
-  <si>
-    <t>9601</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Suspend</t>
-  </si>
-  <si>
-    <t>01/01/2021</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_020</t>
-  </si>
-  <si>
-    <t>TC_CW_020</t>
-  </si>
-  <si>
-    <t>TC_CW_021</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_021</t>
-  </si>
-  <si>
-    <t>TC_CW_022</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_022</t>
-  </si>
-  <si>
-    <t>Close SO</t>
-  </si>
-  <si>
-    <t>TC_CW_023</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_023</t>
-  </si>
-  <si>
-    <t>7250</t>
-  </si>
-  <si>
-    <t>CANCEL TRX</t>
-  </si>
-  <si>
-    <t>Number Of ChequeBook</t>
-  </si>
-  <si>
-    <t>Cheque Code</t>
-  </si>
-  <si>
-    <t>account Branch Code</t>
-  </si>
-  <si>
-    <t>Account Currency Code</t>
-  </si>
-  <si>
-    <t>Account Gl code</t>
-  </si>
-  <si>
-    <t>Account CIF Code</t>
-  </si>
-  <si>
-    <t>Account Serial Number</t>
-  </si>
-  <si>
-    <t>ChequeBook Request Number</t>
-  </si>
-  <si>
-    <t>ChequeFrom Number</t>
-  </si>
-  <si>
-    <t>ChequeFrom To Number</t>
-  </si>
-  <si>
-    <t>TC_CW_002</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_002</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>037</t>
-  </si>
-  <si>
-    <t>CHB_081</t>
-  </si>
-  <si>
-    <t>DS01_TC_CHB_081</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>96123</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>TestCaseID</t>
-  </si>
-  <si>
-    <t>Data Set ID</t>
-  </si>
-  <si>
-    <t>ExecuteYes/No</t>
-  </si>
-  <si>
-    <t>Dependent Test Case Id_One</t>
-  </si>
-  <si>
-    <t>Dependent Test Case Id_Two</t>
-  </si>
-  <si>
-    <t>Dependent Test Case Id_Three</t>
-  </si>
-  <si>
-    <t>Dependent Test Case Id_Four</t>
-  </si>
-  <si>
-    <t>Dependent Test Case Id_Five</t>
-  </si>
-  <si>
-    <t>Dependent Data Set Id_Five</t>
-  </si>
-  <si>
-    <t>CW_001</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>CW_002</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>CW_003</t>
-  </si>
-  <si>
-    <t>CW_004</t>
-  </si>
-  <si>
-    <t>CW_005</t>
-  </si>
-  <si>
-    <t>CW_006</t>
-  </si>
-  <si>
-    <t>CW_007</t>
-  </si>
-  <si>
-    <t>CW_019</t>
-  </si>
-  <si>
-    <t>CW_020</t>
-  </si>
-  <si>
-    <t>CW_021</t>
-  </si>
-  <si>
-    <t>CW_022</t>
-  </si>
-  <si>
-    <t>CW_023</t>
-  </si>
-  <si>
-    <t>CW_024</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_024</t>
-  </si>
-  <si>
-    <t>CW_025</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_025</t>
-  </si>
-  <si>
-    <t>CW_026</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_026</t>
-  </si>
-  <si>
-    <t>CW_038</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_038</t>
-  </si>
-  <si>
-    <t>CW_039</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_039</t>
-  </si>
-  <si>
-    <t>CW_040</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_040</t>
-  </si>
-  <si>
-    <t>CW_041</t>
-  </si>
-  <si>
-    <t>DS01_TC_CW_041</t>
-  </si>
-  <si>
-    <t>Certificate Type</t>
-  </si>
-  <si>
-    <t>CIF Number</t>
-  </si>
-  <si>
-    <t>Number Of Bills</t>
-  </si>
-  <si>
-    <t>Total Amount Of Bills</t>
-  </si>
-  <si>
-    <t>Passbook Code</t>
-  </si>
-  <si>
-    <t>Passbook Type</t>
-  </si>
-  <si>
-    <t>01/01/2017</t>
-  </si>
-  <si>
-    <t>01/01/2023</t>
-  </si>
-  <si>
-    <t>7194</t>
-  </si>
-  <si>
-    <t>7195</t>
-  </si>
-  <si>
-    <t>7192</t>
-  </si>
-  <si>
     <t>01/01/2018</t>
   </si>
   <si>
@@ -704,58 +808,33 @@
     <t>7847</t>
   </si>
   <si>
-    <t>7281</t>
-  </si>
-  <si>
-    <t>7283</t>
-  </si>
-  <si>
-    <t>7284</t>
-  </si>
-  <si>
-    <t>7285</t>
-  </si>
-  <si>
-    <t>7286</t>
-  </si>
-  <si>
-    <t>7287</t>
-  </si>
-  <si>
-    <t>7288</t>
-  </si>
-  <si>
-    <t>7289</t>
-  </si>
-  <si>
-    <t>7290</t>
-  </si>
-  <si>
-    <t>7291</t>
-  </si>
-  <si>
-    <t>7292</t>
-  </si>
-  <si>
-    <t>7293</t>
-  </si>
-  <si>
-    <t>7294</t>
-  </si>
-  <si>
-    <t>7295</t>
+    <t>1018</t>
+  </si>
+  <si>
+    <t>1019</t>
+  </si>
+  <si>
+    <t>1020</t>
+  </si>
+  <si>
+    <t>1021</t>
+  </si>
+  <si>
+    <t>1022</t>
+  </si>
+  <si>
+    <t>1023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="177" formatCode="$#,##0;[RED]-$#,##0"/>
-    <numFmt numFmtId="178" formatCode="$#,##0.00;[RED]-$#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00;[RED]-&quot;$&quot;#,##0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="$#,##0.00;[RED]-$#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;[RED]-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -763,8 +842,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
@@ -778,6 +858,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -833,7 +918,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,12 +981,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -933,6 +1012,16 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -941,18 +1030,8 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -976,12 +1055,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
@@ -1000,188 +1079,124 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="30" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="30" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="30" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="26" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1189,12 +1204,36 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="18">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
     <cellStyle name="Currency" xfId="16" builtinId="4"/>
@@ -1207,31 +1246,12 @@
     <cellStyle name="Heading1" xfId="23"/>
     <cellStyle name="Excel_5f_20_5f_Built-in_5f_20_5f_Normal" xfId="24"/>
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="25"/>
-    <cellStyle name="Excel_5f_5f_5f_20_5f_5f_5f_Built-in_5f_5f_5f_20_5f_5f_5f_Normal" xfId="26"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="27"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="28"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="29"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="30"/>
-    <cellStyle name="Heading_20_1" xfId="31"/>
-    <cellStyle name="Heading1_20_1" xfId="32"/>
-    <cellStyle name="Heading1_5f_20_5f_1" xfId="33"/>
-    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="34"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="35"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="36"/>
-    <cellStyle name="Heading_5f_20_5f_1" xfId="37"/>
-    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="38"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="39"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="40"/>
-    <cellStyle name="Result_20_1" xfId="41"/>
-    <cellStyle name="Result2_20_1" xfId="42"/>
-    <cellStyle name="Result2_5f_20_5f_1" xfId="43"/>
-    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="44"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="45"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="46"/>
-    <cellStyle name="Result_5f_20_5f_1" xfId="47"/>
-    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="48"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="49"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="50"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="26"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="27"/>
+    <cellStyle name="Heading_20_1" xfId="28"/>
+    <cellStyle name="Heading1_20_1" xfId="29"/>
+    <cellStyle name="Result_20_1" xfId="30"/>
+    <cellStyle name="Result2_20_1" xfId="31"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1608,21 +1628,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7548b7a2-c90c-4da8-a333-4f86816a9c5e}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896ccd7f-cac6-4e21-a748-4389f6d1cc28}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="58.857142857142854" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="46.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="38.857142857142854" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="45.714285714285715" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="51.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="62.285714285714285" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="48.57142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="41.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -1660,132 +1680,406 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899189f4-eb3a-4087-af59-6cb3f9033683}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9fe1f306-e94b-40fc-a2be-51b96ec652b5}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.144285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="12.854285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="33" width="15.714285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="33" width="33.285714285714285" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="33" width="37.42857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="33" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="33" width="39.857142857142854" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="33" width="40.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="33" width="43.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="33" width="51.42857142857143" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="33" width="42.42857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="33" width="44.285714285714285" collapsed="true"/>
-    <col min="11" max="16384" style="33" width="12.142857142857142" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="19" width="16.571428571428573" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="19" width="35.142857142857146" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="19" width="39.57142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="19" width="15.714285714285714" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="19" width="42.142857142857146" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="19" width="42.285714285714285" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="19" width="45.42857142857143" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="19" width="54.285714285714285" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="19" width="44.857142857142854" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="19" width="46.857142857142854" collapsed="true"/>
+    <col min="11" max="16384" style="19" width="12.857142857142858" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.05">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="29" t="s">
+      <c r="D2" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.05">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.05">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.05">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.05">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.05">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.05">
+      <c r="A8" s="27">
+        <v>7</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.05">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+    </row>
+    <row r="10" spans="1:10" ht="14.05">
+      <c r="A10" s="27">
+        <v>9</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.05">
+      <c r="A11" s="27">
+        <v>10</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.05">
+      <c r="A12" s="27">
+        <v>11</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="23" t="s">
+      <c r="C12" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.05">
+      <c r="A13" s="27">
+        <v>12</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+    </row>
+    <row r="14" spans="1:10" ht="14.05">
+      <c r="A14" s="27">
+        <v>13</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.05">
+      <c r="A15" s="27">
+        <v>14</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.05">
-      <c r="A2" s="24">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="30" t="s">
+      <c r="C15" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.05">
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="D16" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="2.5209" bottom="2.5209" header="2.324" footer="2.324"/>
+  <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0fcb91a7-4370-4f07-acdc-f23d543726ed}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376b12a9-9432-4806-a911-de8119abf234}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.424285714285714" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="12.144285714285713" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="33" width="41.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="33" width="43.285714285714285" collapsed="true"/>
-    <col min="3" max="9" customWidth="true" style="33" width="32.857142857142854" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="33" width="36.142857142857146" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="33" width="41.42857142857143" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="33" width="40.57142857142857" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="33" width="32.142857142857146" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="33" width="31.571428571428573" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="33" width="36.714285714285715" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="33" width="40.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="33" width="33.285714285714285" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="33" width="26.571428571428573" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="33" width="30.142857142857142" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="33" width="43.714285714285715" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="33" width="43.285714285714285" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="33" width="42.857142857142854" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="33" width="43.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="33" width="41.285714285714285" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="33" width="31.142857142857142" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="33" width="39.285714285714285" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="33" width="24.857142857142858" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="33" width="35.857142857142854" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="33" width="27.0" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="33" width="22.714285714285715" collapsed="true"/>
-    <col min="31" max="16384" style="33" width="11.428571428571429" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="19" width="43.285714285714285" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="19" width="45.714285714285715" collapsed="true"/>
+    <col min="3" max="9" customWidth="true" style="19" width="34.714285714285715" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="19" width="38.142857142857146" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="19" width="43.714285714285715" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="19" width="42.857142857142854" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="19" width="34.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="19" width="33.285714285714285" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="19" width="38.714285714285715" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="19" width="42.285714285714285" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="19" width="35.142857142857146" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="19" width="28.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="19" width="31.857142857142858" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="19" width="46.142857142857146" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="19" width="45.714285714285715" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="19" width="45.285714285714285" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="19" width="45.42857142857143" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="19" width="43.57142857142857" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="19" width="32.857142857142854" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="19" width="41.42857142857143" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="19" width="26.285714285714285" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="19" width="37.857142857142854" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="19" width="28.571428571428573" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="19" width="24.0" collapsed="true"/>
+    <col min="31" max="16384" style="19" width="12.142857142857142" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.05">
@@ -1796,22 +2090,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>82</v>
@@ -1931,10 +2225,10 @@
       </c>
       <c r="AA2" s="15"/>
       <c r="AB2" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC2" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD2" s="18"/>
     </row>
@@ -1980,7 +2274,7 @@
         <v>110</v>
       </c>
       <c r="U3" s="17" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
@@ -1991,10 +2285,10 @@
       </c>
       <c r="AA3" s="15"/>
       <c r="AB3" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC3" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD3" s="18"/>
     </row>
@@ -2048,7 +2342,7 @@
         <v>110</v>
       </c>
       <c r="U4" s="17" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
@@ -2059,10 +2353,10 @@
       </c>
       <c r="AA4" s="15"/>
       <c r="AB4" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC4" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD4" s="18"/>
     </row>
@@ -2108,7 +2402,7 @@
         <v>110</v>
       </c>
       <c r="U5" s="17" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
@@ -2119,10 +2413,10 @@
       </c>
       <c r="AA5" s="15"/>
       <c r="AB5" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC5" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD5" s="18"/>
     </row>
@@ -2177,19 +2471,19 @@
       </c>
       <c r="AA6" s="15"/>
       <c r="AB6" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC6" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD6" s="18"/>
     </row>
     <row r="7" spans="1:30" ht="12.8">
       <c r="A7" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -2226,7 +2520,7 @@
         <v>110</v>
       </c>
       <c r="U7" s="17" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
@@ -2237,19 +2531,19 @@
       </c>
       <c r="AA7" s="15"/>
       <c r="AB7" s="15" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="AC7" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD7" s="18"/>
     </row>
     <row r="8" spans="1:30" ht="12.8">
       <c r="A8" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -2258,7 +2552,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J8" s="15" t="s">
         <v>63</v>
@@ -2282,7 +2576,7 @@
         <v>63</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R8" s="15" t="s">
         <v>39</v>
@@ -2295,10 +2589,10 @@
       </c>
       <c r="U8" s="17"/>
       <c r="V8" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W8" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
@@ -2306,24 +2600,24 @@
         <v>111</v>
       </c>
       <c r="AA8" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB8" s="15" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="AC8" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD8" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="12.8">
       <c r="A9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -2358,10 +2652,10 @@
     </row>
     <row r="10" spans="1:30" ht="12.8">
       <c r="A10" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -2370,7 +2664,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>63</v>
@@ -2394,7 +2688,7 @@
         <v>63</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>39</v>
@@ -2407,7 +2701,7 @@
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
@@ -2416,22 +2710,22 @@
         <v>111</v>
       </c>
       <c r="AA10" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB10" s="15" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="AC10" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="1:30" ht="12.8">
       <c r="A11" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -2440,7 +2734,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>63</v>
@@ -2464,7 +2758,7 @@
         <v>63</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R11" s="15" t="s">
         <v>39</v>
@@ -2477,33 +2771,33 @@
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W11" s="15"/>
       <c r="X11" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Y11" s="15"/>
       <c r="Z11" s="18" t="s">
         <v>111</v>
       </c>
       <c r="AA11" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="AC11" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD11" s="18"/>
     </row>
     <row r="12" spans="1:30" ht="12.8">
       <c r="A12" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -2512,7 +2806,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J12" s="15" t="s">
         <v>63</v>
@@ -2536,7 +2830,7 @@
         <v>63</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R12" s="15" t="s">
         <v>39</v>
@@ -2548,48 +2842,48 @@
         <v>110</v>
       </c>
       <c r="U12" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V12" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Z12" s="18" t="s">
         <v>111</v>
       </c>
       <c r="AA12" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB12" s="15" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="AC12" s="15" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="AD12" s="18"/>
     </row>
     <row r="13" spans="1:30" ht="12.8">
       <c r="A13" s="12" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2618,22 +2912,22 @@
     </row>
     <row r="14" spans="1:30" ht="12.8">
       <c r="A14" s="12" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
@@ -2661,21 +2955,21 @@
       <c r="AD14" s="18"/>
     </row>
     <row r="15" spans="1:30" ht="12.8">
-      <c r="A15" s="34" t="s">
-        <v>220</v>
+      <c r="A15" s="20" t="s">
+        <v>244</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15" t="s">
@@ -2685,7 +2979,7 @@
         <v>37</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="M15" s="15" t="s">
         <v>39</v>
@@ -2711,21 +3005,21 @@
       <c r="AD15" s="18"/>
     </row>
     <row r="16" spans="1:30" ht="12.8">
-      <c r="A16" s="34" t="s">
-        <v>224</v>
+      <c r="A16" s="20" t="s">
+        <v>248</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15" t="s">
@@ -2735,7 +3029,7 @@
         <v>37</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="M16" s="15" t="s">
         <v>39</v>
@@ -2761,27 +3055,27 @@
       <c r="AD16" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.226" bottom="2.226" header="2.0291" footer="2.0291"/>
+  <pageMargins left="0.7" right="0.7" top="2.5209" bottom="2.5209" header="2.324" footer="2.324"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126b1998-9c8d-4d23-934a-66bd5273ec14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20eefe90-a926-41eb-bc6a-63a236d863a5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="40.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="48.714285714285715" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="46.857142857142854" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="59.285714285714285" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="74.57142857142857" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="42.285714285714285" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="51.42857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="49.57142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="62.714285714285715" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="78.85714285714286" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -2819,25 +3113,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354ff782-d33d-43f7-a723-866b68bac39c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{eff01bc6-c443-4e1b-9b44-9c8ebd743b31}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" style="3" width="20.428571428571427" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="71.71428571428571" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="63.714285714285715" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="75.85714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="67.28571428571429" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.05">
@@ -2863,30 +3157,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e2eca647-ef80-4142-8f6d-a20f8e4b1e41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ee7b053-8328-4b0d-b612-4f1b27b16d9a}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="54.42857142857143" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="81.57142857142857" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="63.142857142857146" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="55.857142857142854" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="53.42857142857143" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="45.285714285714285" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="57.57142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="86.28571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="66.71428571428571" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="59.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="51.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="56.42857142857143" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="3" width="51.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="47.857142857142854" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.05">
@@ -3035,30 +3329,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931d571e-331b-44ec-9884-d8efa1443745}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3f5e5cec-56bb-4ca4-8469-5bcbbc5365e6}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="75.28571428571429" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="105.28571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="57.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="74.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="70.14285714285714" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="54.42857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="62.714285714285715" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="83.42857142857143" collapsed="true"/>
-    <col min="9" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="79.57142857142857" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="111.28571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="60.285714285714285" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="78.28571428571429" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="74.14285714285714" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="57.57142857142857" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="66.28571428571429" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="88.14285714285714" collapsed="true"/>
+    <col min="9" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.05">
@@ -3244,31 +3538,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1f64f7ee-c8ba-40ad-9d01-a4be313a85c7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d3f40ae2-e92a-44a2-b510-7b67d542c023}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.424285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="49.57142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="64.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="61.857142857142854" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="60.285714285714285" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="37.857142857142854" collapsed="true"/>
-    <col min="6" max="7" style="3" width="20.428571428571427" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="3" width="52.42857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="34.42857142857143" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="42.285714285714285" collapsed="true"/>
-    <col min="12" max="16384" style="3" width="20.428571428571427" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="3" width="52.42857142857143" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="67.71428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="65.42857142857143" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="63.714285714285715" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="40.0" collapsed="true"/>
+    <col min="6" max="7" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="3" width="55.42857142857143" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="36.42857142857143" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="44.714285714285715" collapsed="true"/>
+    <col min="12" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -3307,10 +3601,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.05">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -3337,13 +3631,13 @@
       <c r="J2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="10"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="14.05">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -3370,13 +3664,13 @@
       <c r="J3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="14.05">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -3403,68 +3697,68 @@
       <c r="J4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{cfbac0fc-20df-4ff0-a18e-96fdb2c1671a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40354208-95a7-41e5-898c-f6e8df345417}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="S1">
+    <sheetView workbookViewId="0" topLeftCell="S1">
       <selection pane="topLeft" activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.284285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="21.424285714285716" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="40.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="59.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="65.28571428571429" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="43.57142857142857" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="13" width="64.28571428571429" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="53.42857142857143" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="13" width="48.142857142857146" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="59.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="13" width="51.42857142857143" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="13" width="45.714285714285715" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="13" width="44.714285714285715" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="13" width="40.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="13" width="19.1328125" collapsed="true"/>
-    <col min="16" max="20" customWidth="true" style="13" width="43.714285714285715" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" style="13" width="30.857142857142858" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" style="13" width="50.285714285714285" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="13" width="36.142857142857146" collapsed="true"/>
-    <col min="26" max="16384" style="13" width="20.285714285714285" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="13" width="62.42857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="13" width="69.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="13" width="46.0" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="13" width="68.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="56.42857142857143" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="13" width="50.857142857142854" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="13" width="62.42857142857143" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="13" width="54.285714285714285" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="13" width="48.285714285714285" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="13" width="47.285714285714285" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="13" width="20.142857142857142" collapsed="true"/>
+    <col min="16" max="20" customWidth="true" style="13" width="46.142857142857146" collapsed="true"/>
+    <col min="21" max="22" customWidth="true" style="13" width="32.57142857142857" collapsed="true"/>
+    <col min="23" max="24" customWidth="true" style="13" width="53.142857142857146" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="13" width="38.142857142857146" collapsed="true"/>
+    <col min="26" max="16384" style="13" width="21.428571428571427" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.05">
@@ -3635,7 +3929,7 @@
         <v>110</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>235</v>
+        <v>116</v>
       </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
@@ -3700,7 +3994,7 @@
         <v>110</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
@@ -3757,7 +4051,7 @@
         <v>110</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
@@ -3814,7 +4108,7 @@
         <v>110</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
@@ -3837,10 +4131,10 @@
     </row>
     <row r="7" spans="1:25" ht="12.8">
       <c r="A7" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>107</v>
@@ -3871,7 +4165,7 @@
         <v>110</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>239</v>
+        <v>130</v>
       </c>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
@@ -3894,13 +4188,13 @@
     </row>
     <row r="8" spans="1:25" ht="12.8">
       <c r="A8" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>63</v>
@@ -3924,7 +4218,7 @@
         <v>63</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>39</v>
@@ -3937,10 +4231,10 @@
       </c>
       <c r="O8" s="17"/>
       <c r="P8" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
@@ -3948,7 +4242,7 @@
         <v>111</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="V8" s="15" t="s">
         <v>22</v>
@@ -3960,15 +4254,15 @@
         <v>113</v>
       </c>
       <c r="Y8" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="12.8">
       <c r="A9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -3998,13 +4292,13 @@
     </row>
     <row r="10" spans="1:25" ht="12.8">
       <c r="A10" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>63</v>
@@ -4028,7 +4322,7 @@
         <v>63</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>39</v>
@@ -4041,7 +4335,7 @@
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
@@ -4065,13 +4359,13 @@
     </row>
     <row r="11" spans="1:25" ht="12.8">
       <c r="A11" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>63</v>
@@ -4095,7 +4389,7 @@
         <v>63</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>39</v>
@@ -4108,11 +4402,11 @@
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q11" s="15"/>
       <c r="R11" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="18" t="s">
@@ -4134,13 +4428,13 @@
     </row>
     <row r="12" spans="1:25" ht="12.8">
       <c r="A12" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>63</v>
@@ -4164,7 +4458,7 @@
         <v>63</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>39</v>
@@ -4176,15 +4470,15 @@
         <v>110</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="T12" s="18" t="s">
         <v>111</v>
@@ -4204,578 +4498,733 @@
       <c r="Y12" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25f8a1e8-a6fb-4fe5-a4c2-9945522a1a5b}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ae20eb1c-647f-4bfc-b26e-dd7391c19518}">
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.284285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="21.424285714285716" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="37.142857142857146" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="63.142857142857146" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="55.42857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="48.714285714285715" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="13" width="58.857142857142854" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="13" width="57.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="40.57142857142857" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="13" width="50.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="13" width="48.57142857142857" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="39.57142857142857" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="13" width="26.285714285714285" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="13" width="32.42857142857143" collapsed="true"/>
-    <col min="13" max="16384" style="13" width="20.285714285714285" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="13" width="39.285714285714285" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="13" width="66.71428571428571" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="16.1796875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="13" width="58.57142857142857" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="51.42857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="62.285714285714285" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="13" width="60.285714285714285" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="13" width="42.857142857142854" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="13" width="52.857142857142854" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="13" width="51.285714285714285" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="13" width="41.857142857142854" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="13" width="27.714285714285715" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="13" width="34.285714285714285" collapsed="true"/>
+    <col min="15" max="16384" style="13" width="21.428571428571427" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.05">
+    <row r="1" spans="1:14" ht="14.05">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>149</v>
       </c>
+      <c r="D1" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="E1" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="I1" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="J1" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="K1" s="23" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="12.8">
+      <c r="L1" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="12.8">
       <c r="A2" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="15">
+        <v>162</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="24" t="s">
+        <v>164</v>
+      </c>
       <c r="L2" s="22"/>
-    </row>
-    <row r="3" spans="1:12" ht="12.8">
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.8">
       <c r="A3" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="15">
+        <v>166</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>165</v>
-      </c>
       <c r="H3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="K3" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
       <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.1">
+      <c r="A4" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.1">
+      <c r="A5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" ht="12.8">
+      <c r="A6" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" ht="12.8">
+      <c r="A7" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{aae75a31-f5d7-4470-b0ba-d14ce2bead6c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021ea185-1ac1-4344-9b58-55fe8cb6020b}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.284285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="19.284285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="25" width="19.428571428571427" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="25" width="97.28571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="25" width="73.71428571428571" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="25" width="14.92578125" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" style="25" width="85.14285714285714" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="25" width="57.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="25" width="56.42857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="25" width="54.42857142857143" collapsed="true"/>
-    <col min="11" max="16384" style="32" width="18.285714285714285" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="28" width="20.428571428571427" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="28" width="102.85714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="28" width="77.85714285714286" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="28" width="15.714285714285714" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" style="28" width="90.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="28" width="60.285714285714285" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="28" width="59.714285714285715" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="28" width="57.57142857142857" collapsed="true"/>
+    <col min="11" max="16384" style="13" width="19.285714285714285" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
-      <c r="A1" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>175</v>
+      <c r="A1" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
-      <c r="A2" s="24">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="14.05">
-      <c r="A3" s="24">
+      <c r="A3" s="27">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="B3" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="14.05">
-      <c r="A4" s="24">
+      <c r="A4" s="27">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="D4" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="24">
+      <c r="A5" s="27">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="D5" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="24">
+      <c r="A6" s="27">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="D6" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="14.05">
-      <c r="A7" s="24">
+      <c r="A7" s="27">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="D7" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="14.05">
-      <c r="A8" s="24">
+      <c r="A8" s="27">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
+      <c r="B8" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="14.05">
-      <c r="A9" s="24">
+      <c r="A9" s="27">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="B9" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="14.05">
-      <c r="A10" s="24">
+      <c r="A10" s="27">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+      <c r="B10" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="14.05">
-      <c r="A11" s="24">
+      <c r="A11" s="27">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="B11" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="14.05">
-      <c r="A12" s="24">
+      <c r="A12" s="27">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="B12" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="14.05">
-      <c r="A13" s="24">
+      <c r="A13" s="27">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="14.05">
-      <c r="A14" s="24">
+      <c r="A14" s="27">
         <v>13</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="B14" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="14.05">
-      <c r="A15" s="24">
+      <c r="A15" s="27">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="B15" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="14.05">
-      <c r="A16" s="24">
+      <c r="A16" s="27">
         <v>15</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="B16" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="14.05">
-      <c r="A17" s="24">
+      <c r="A17" s="27">
         <v>16</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="B17" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="14.05">
-      <c r="A18" s="24">
+      <c r="A18" s="27">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+      <c r="B18" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="14.05">
-      <c r="A19" s="24">
+      <c r="A19" s="27">
         <v>18</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="B19" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10" ht="14.05">
-      <c r="A20" s="24">
+      <c r="A20" s="27">
         <v>19</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="B20" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Commit on 12 may 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="CSM_Login" sheetId="1" r:id="rId3"/>
-    <sheet name="CSMParam_login" sheetId="2" r:id="rId4"/>
-    <sheet name="SadsLogin" sheetId="3" r:id="rId5"/>
-    <sheet name="CSM_ClientProcessingStatement" sheetId="4" r:id="rId6"/>
-    <sheet name="CSM_LostAndFoundManagement" sheetId="5" r:id="rId7"/>
-    <sheet name="AmendChequeCardStatusTestData" sheetId="6" r:id="rId8"/>
-    <sheet name="CSM_Transaction" sheetId="7" r:id="rId9"/>
-    <sheet name="CSM_ChequeBookrequest" sheetId="8" r:id="rId10"/>
-    <sheet name="ChargeWaiverExecutionTracker" sheetId="9" r:id="rId11"/>
-    <sheet name="CheuqeBookRequestExecutionTrack" sheetId="10" r:id="rId12"/>
-    <sheet name="CSM_ChargeWaiverTestData" sheetId="11" r:id="rId13"/>
+    <sheet name="CSM_Login" sheetId="1" r:id="rId1"/>
+    <sheet name="CSMParam_login" sheetId="2" r:id="rId2"/>
+    <sheet name="SadsLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="CSM_ClientProcessingStatement" sheetId="4" r:id="rId4"/>
+    <sheet name="CSM_LostAndFoundManagement" sheetId="5" r:id="rId5"/>
+    <sheet name="AmendChequeCardStatusTestData" sheetId="6" r:id="rId6"/>
+    <sheet name="CSM_Transaction" sheetId="7" r:id="rId7"/>
+    <sheet name="CSM_ChequeBookrequest" sheetId="8" r:id="rId8"/>
+    <sheet name="ChargeWaiverExecutionTracker" sheetId="9" r:id="rId9"/>
+    <sheet name="CheuqeBookRequestExecutionTrack" sheetId="10" r:id="rId10"/>
+    <sheet name="CSM_ChargeWaiverTestData" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="272">
   <si>
     <t>Stage</t>
   </si>
@@ -531,6 +531,31 @@
   </si>
   <si>
     <t>96123</t>
+  </si>
+  <si>
+    <t>CHB_119_120_Prereq_01</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DS01_TC_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>CHB_119_120_Prereq_01</t>
+    </r>
+  </si>
+  <si>
+    <t>124</t>
   </si>
   <si>
     <t>CHB_123_124_Prereq_01</t>
@@ -555,9 +580,6 @@
     </r>
   </si>
   <si>
-    <t>124</t>
-  </si>
-  <si>
     <t>CHB_123_124_Prereq_02</t>
   </si>
   <si>
@@ -688,27 +710,6 @@
   </si>
   <si>
     <t>DS01_TC_CW_041</t>
-  </si>
-  <si>
-    <t>CHB_112</t>
-  </si>
-  <si>
-    <t>CHB_113</t>
-  </si>
-  <si>
-    <t>CHB_119</t>
-  </si>
-  <si>
-    <t>CHB_120</t>
-  </si>
-  <si>
-    <t>CHB_121</t>
-  </si>
-  <si>
-    <t>ChequeBookPrerequisites_01</t>
-  </si>
-  <si>
-    <t>CHB_123_124_Prereq</t>
   </si>
   <si>
     <r>
@@ -730,9 +731,6 @@
     </r>
   </si>
   <si>
-    <t>CHB_122</t>
-  </si>
-  <si>
     <t>ChequeBookPrerequisites_02</t>
   </si>
   <si>
@@ -808,33 +806,98 @@
     <t>7847</t>
   </si>
   <si>
-    <t>1018</t>
-  </si>
-  <si>
-    <t>1019</t>
-  </si>
-  <si>
-    <t>1020</t>
-  </si>
-  <si>
-    <t>1021</t>
-  </si>
-  <si>
-    <t>1022</t>
-  </si>
-  <si>
-    <t>1023</t>
+    <t>CHB_119_120_121_Prereq_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_119_120_121_Prereq_01</t>
+  </si>
+  <si>
+    <t>CHB_119_120_121_Prereq_02</t>
+  </si>
+  <si>
+    <t>CHB_119_120_121_Prereq_03</t>
+  </si>
+  <si>
+    <t>DS01_CHB_119_120_121_Prereq_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_119_120_121_Prereq_03</t>
+  </si>
+  <si>
+    <t>CSB_120_01</t>
+  </si>
+  <si>
+    <t>CSB_120_02</t>
+  </si>
+  <si>
+    <t>DS01_CSB_120_01</t>
+  </si>
+  <si>
+    <t>CHB_119_01</t>
+  </si>
+  <si>
+    <t>CHB_119_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_119_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_119_02</t>
+  </si>
+  <si>
+    <t>DS01_CSB_120_02</t>
+  </si>
+  <si>
+    <t>CSB_121_01</t>
+  </si>
+  <si>
+    <t>CSB_121_02</t>
+  </si>
+  <si>
+    <t>DS01_CSB_121_01</t>
+  </si>
+  <si>
+    <t>DS01_CSB_121_02</t>
+  </si>
+  <si>
+    <t>CHB_112_113_Prereq_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_112_113_Prereq_01</t>
+  </si>
+  <si>
+    <t>CHB_112_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_112_01</t>
+  </si>
+  <si>
+    <t>CHB_112_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_112_02</t>
+  </si>
+  <si>
+    <t>CHB_113_01</t>
+  </si>
+  <si>
+    <t>CHB_113_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_113_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_113_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="$#,##0.00;[RED]-$#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;[RED]-&quot;$&quot;#,##0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -886,23 +949,6 @@
     <font>
       <b/>
       <i/>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -911,7 +957,7 @@
     <font>
       <b/>
       <i/>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1007,6 +1053,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1017,6 +1064,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1029,298 +1077,77 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+  <cellStyleXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="27" applyNumberFormat="1" applyFont="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="26" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment/>
-      <protection/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="8">
+    <cellStyle name="Excel_20_Built-in_20_Normal" xfId="5"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="6"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="7"/>
+    <cellStyle name="Heading" xfId="3"/>
+    <cellStyle name="Heading1" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
-    <cellStyle name="Result" xfId="20"/>
-    <cellStyle name="Result2" xfId="21"/>
-    <cellStyle name="Heading" xfId="22"/>
-    <cellStyle name="Heading1" xfId="23"/>
-    <cellStyle name="Excel_5f_20_5f_Built-in_5f_20_5f_Normal" xfId="24"/>
-    <cellStyle name="Excel_20_Built-in_20_Normal" xfId="25"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="26"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="27"/>
-    <cellStyle name="Heading_20_1" xfId="28"/>
-    <cellStyle name="Heading1_20_1" xfId="29"/>
-    <cellStyle name="Result_20_1" xfId="30"/>
-    <cellStyle name="Result2_20_1" xfId="31"/>
+    <cellStyle name="Result" xfId="1"/>
+    <cellStyle name="Result2" xfId="2"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1375,7 +1202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1427,7 +1254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1621,31 +1448,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896ccd7f-cac6-4e21-a748-4389f6d1cc28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="51.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="62.285714285714285" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="48.57142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="41.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="48.285714285714285" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="51" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="62.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="48.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="48.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.05">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.05">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1680,67 +1505,67 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9fe1f306-e94b-40fc-a2be-51b96ec652b5}">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.854285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="19" width="16.571428571428573" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="19" width="35.142857142857146" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="19" width="39.57142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="19" width="15.714285714285714" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="19" width="42.142857142857146" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="19" width="42.285714285714285" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="19" width="45.42857142857143" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="19" width="54.285714285714285" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="19" width="44.857142857142854" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="19" width="46.857142857142854" collapsed="true"/>
-    <col min="11" max="16384" style="19" width="12.857142857142858" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" style="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" style="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.5703125" style="19" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="42.140625" style="19" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="45.42578125" style="19" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="54.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="44.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="46.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="12.85546875" style="19" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.05">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="26" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.05">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -1751,7 +1576,7 @@
         <v>166</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
@@ -1760,18 +1585,18 @@
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" ht="14.05">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="27">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>166</v>
+      <c r="B3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -1780,18 +1605,18 @@
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:10" ht="14.05">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="27">
         <v>3</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>166</v>
+      <c r="B4" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>265</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
@@ -1800,18 +1625,18 @@
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" ht="14.05">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="27">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>166</v>
+      <c r="B5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
@@ -1820,18 +1645,18 @@
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
     </row>
-    <row r="6" spans="1:10" ht="14.05">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="27">
         <v>5</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>166</v>
+      <c r="B6" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
@@ -1840,18 +1665,18 @@
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:10" ht="14.05">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="27">
         <v>6</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>166</v>
+      <c r="B7" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
@@ -1860,16 +1685,18 @@
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" ht="14.05">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="27">
         <v>7</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" s="31"/>
+      <c r="B8" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>271</v>
+      </c>
       <c r="D8" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
@@ -1878,18 +1705,18 @@
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" ht="14.05">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="27">
         <v>8</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>223</v>
+      <c r="B9" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>245</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
@@ -1898,18 +1725,18 @@
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" ht="14.05">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="27">
         <v>9</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>166</v>
+      <c r="B10" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>255</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
@@ -1918,16 +1745,18 @@
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
     </row>
-    <row r="11" spans="1:10" ht="14.05">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="27">
         <v>10</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11" s="31"/>
+      <c r="B11" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>256</v>
+      </c>
       <c r="D11" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
@@ -1936,18 +1765,18 @@
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
     </row>
-    <row r="12" spans="1:10" ht="14.05">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="27">
         <v>11</v>
       </c>
-      <c r="B12" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>223</v>
+      <c r="B12" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -1956,18 +1785,18 @@
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" ht="14.05">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="27">
         <v>12</v>
       </c>
-      <c r="B13" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>174</v>
+      <c r="B13" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>252</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -1976,16 +1805,18 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
     </row>
-    <row r="14" spans="1:10" ht="14.05">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="27">
         <v>13</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C14" s="31"/>
+      <c r="B14" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="D14" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
@@ -1994,18 +1825,18 @@
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="14.05">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="27">
         <v>14</v>
       </c>
-      <c r="B15" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>223</v>
+      <c r="B15" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>249</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
@@ -2014,18 +1845,18 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="14.05">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="27">
         <v>15</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>177</v>
+      <c r="B16" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>260</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
@@ -2034,55 +1865,191 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
     </row>
+    <row r="17" spans="1:10" ht="15">
+      <c r="A17" s="27">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="1:10" ht="15">
+      <c r="A18" s="27">
+        <v>17</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="1:10" ht="15">
+      <c r="A19" s="27">
+        <v>18</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+    </row>
+    <row r="20" spans="1:10" ht="15">
+      <c r="A20" s="27">
+        <v>19</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+    </row>
+    <row r="21" spans="1:10" ht="15">
+      <c r="A21" s="27">
+        <v>20</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+    </row>
+    <row r="22" spans="1:10" ht="15">
+      <c r="A22" s="27">
+        <v>21</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+    </row>
+    <row r="23" spans="1:10" ht="15">
+      <c r="A23" s="27">
+        <v>22</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="2.8162000000000003" bottom="2.8162000000000003" header="2.6193" footer="2.6193"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376b12a9-9432-4806-a911-de8119abf234}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.144285714285713" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="19" width="43.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="19" width="45.714285714285715" collapsed="true"/>
-    <col min="3" max="9" customWidth="true" style="19" width="34.714285714285715" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="19" width="38.142857142857146" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="19" width="43.714285714285715" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="19" width="42.857142857142854" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="19" width="34.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="19" width="33.285714285714285" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="19" width="38.714285714285715" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="19" width="42.285714285714285" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="19" width="35.142857142857146" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="19" width="28.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="19" width="31.857142857142858" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="19" width="46.142857142857146" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="19" width="45.714285714285715" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="19" width="45.285714285714285" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="19" width="45.42857142857143" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="19" width="43.57142857142857" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="19" width="32.857142857142854" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="19" width="41.42857142857143" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="19" width="26.285714285714285" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="19" width="37.857142857142854" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="19" width="28.571428571428573" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="19" width="24.0" collapsed="true"/>
-    <col min="31" max="16384" style="19" width="12.142857142857142" collapsed="true"/>
+    <col min="1" max="1" width="43.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="34.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="38.140625" style="19" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="43.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="42.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="34" style="19" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="33.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="38.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="42.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="35.140625" style="19" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28" style="19" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="31.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="46.140625" style="19" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="45.7109375" style="19" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="45.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="45.42578125" style="19" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="43.5703125" style="19" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="32.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="41.42578125" style="19" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="26.28515625" style="19" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="37.85546875" style="19" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="28.5703125" style="19" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="24" style="19" customWidth="1" collapsed="1"/>
+    <col min="31" max="16384" width="12.140625" style="19" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14.05">
+    <row r="1" spans="1:30" ht="15">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -2090,22 +2057,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>82</v>
@@ -2174,7 +2141,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="12.8">
+    <row r="2" spans="1:30">
       <c r="A2" s="12" t="s">
         <v>105</v>
       </c>
@@ -2225,14 +2192,14 @@
       </c>
       <c r="AA2" s="15"/>
       <c r="AB2" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC2" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD2" s="18"/>
     </row>
-    <row r="3" spans="1:30" ht="12.8">
+    <row r="3" spans="1:30">
       <c r="A3" s="12" t="s">
         <v>114</v>
       </c>
@@ -2274,7 +2241,7 @@
         <v>110</v>
       </c>
       <c r="U3" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
@@ -2285,14 +2252,14 @@
       </c>
       <c r="AA3" s="15"/>
       <c r="AB3" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC3" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD3" s="18"/>
     </row>
-    <row r="4" spans="1:30" ht="12.8">
+    <row r="4" spans="1:30">
       <c r="A4" s="12" t="s">
         <v>117</v>
       </c>
@@ -2342,7 +2309,7 @@
         <v>110</v>
       </c>
       <c r="U4" s="17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="V4" s="15"/>
       <c r="W4" s="15"/>
@@ -2353,14 +2320,14 @@
       </c>
       <c r="AA4" s="15"/>
       <c r="AB4" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC4" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD4" s="18"/>
     </row>
-    <row r="5" spans="1:30" ht="12.8">
+    <row r="5" spans="1:30">
       <c r="A5" s="12" t="s">
         <v>122</v>
       </c>
@@ -2402,7 +2369,7 @@
         <v>110</v>
       </c>
       <c r="U5" s="17" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
@@ -2413,14 +2380,14 @@
       </c>
       <c r="AA5" s="15"/>
       <c r="AB5" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC5" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD5" s="18"/>
     </row>
-    <row r="6" spans="1:30" ht="12.8">
+    <row r="6" spans="1:30">
       <c r="A6" s="12" t="s">
         <v>125</v>
       </c>
@@ -2471,14 +2438,14 @@
       </c>
       <c r="AA6" s="15"/>
       <c r="AB6" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC6" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD6" s="18"/>
     </row>
-    <row r="7" spans="1:30" ht="12.8">
+    <row r="7" spans="1:30">
       <c r="A7" s="12" t="s">
         <v>128</v>
       </c>
@@ -2520,7 +2487,7 @@
         <v>110</v>
       </c>
       <c r="U7" s="17" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
@@ -2531,14 +2498,14 @@
       </c>
       <c r="AA7" s="15"/>
       <c r="AB7" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AC7" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD7" s="18"/>
     </row>
-    <row r="8" spans="1:30" ht="12.8">
+    <row r="8" spans="1:30">
       <c r="A8" s="12" t="s">
         <v>131</v>
       </c>
@@ -2603,16 +2570,16 @@
         <v>137</v>
       </c>
       <c r="AB8" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AC8" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD8" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="12.8">
+    <row r="9" spans="1:30">
       <c r="A9" s="12" t="s">
         <v>139</v>
       </c>
@@ -2650,7 +2617,7 @@
       <c r="AC9" s="15"/>
       <c r="AD9" s="18"/>
     </row>
-    <row r="10" spans="1:30" ht="12.8">
+    <row r="10" spans="1:30">
       <c r="A10" s="12" t="s">
         <v>140</v>
       </c>
@@ -2713,14 +2680,14 @@
         <v>137</v>
       </c>
       <c r="AB10" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AC10" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD10" s="18"/>
     </row>
-    <row r="11" spans="1:30" ht="12.8">
+    <row r="11" spans="1:30">
       <c r="A11" s="12" t="s">
         <v>142</v>
       </c>
@@ -2785,14 +2752,14 @@
         <v>137</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AC11" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD11" s="18"/>
     </row>
-    <row r="12" spans="1:30" ht="12.8">
+    <row r="12" spans="1:30">
       <c r="A12" s="12" t="s">
         <v>145</v>
       </c>
@@ -2859,28 +2826,28 @@
         <v>137</v>
       </c>
       <c r="AB12" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AC12" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD12" s="18"/>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="AD12" s="18"/>
-    </row>
-    <row r="13" spans="1:30" ht="12.8">
-      <c r="A13" s="12" t="s">
-        <v>240</v>
-      </c>
       <c r="B13" s="12" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>167</v>
@@ -2910,21 +2877,21 @@
       <c r="AC13" s="15"/>
       <c r="AD13" s="18"/>
     </row>
-    <row r="14" spans="1:30" ht="12.8">
+    <row r="14" spans="1:30">
       <c r="A14" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>167</v>
@@ -2954,22 +2921,22 @@
       <c r="AC14" s="15"/>
       <c r="AD14" s="18"/>
     </row>
-    <row r="15" spans="1:30" ht="12.8">
+    <row r="15" spans="1:30">
       <c r="A15" s="20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="15" t="s">
@@ -2979,7 +2946,7 @@
         <v>37</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="M15" s="15" t="s">
         <v>39</v>
@@ -3004,22 +2971,22 @@
       <c r="AC15" s="15"/>
       <c r="AD15" s="18"/>
     </row>
-    <row r="16" spans="1:30" ht="12.8">
+    <row r="16" spans="1:30">
       <c r="A16" s="20" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15" t="s">
@@ -3029,7 +2996,7 @@
         <v>37</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="M16" s="15" t="s">
         <v>39</v>
@@ -3055,30 +3022,28 @@
       <c r="AD16" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="2.5209" bottom="2.5209" header="2.324" footer="2.324"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="2.5209000000000001" bottom="2.5209000000000001" header="2.3239999999999998" footer="2.3239999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20eefe90-a926-41eb-bc6a-63a236d863a5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="42.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="51.42857142857143" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="49.57142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="62.714285714285715" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="78.85714285714286" collapsed="true"/>
-    <col min="6" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="42.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="62.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="78.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.05">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3095,7 +3060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.05">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3113,28 +3078,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{eff01bc6-c443-4e1b-9b44-9c8ebd743b31}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="3" width="21.571428571428573" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="75.85714285714286" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="67.28571428571429" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" style="3" collapsed="1"/>
+    <col min="2" max="2" width="75.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="67.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.05">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3145,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.05">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3157,33 +3120,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ee7b053-8328-4b0d-b612-4f1b27b16d9a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="57.57142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="86.28571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="66.71428571428571" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="59.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="51.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="56.42857142857143" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="3" width="51.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="47.857142857142854" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="57.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="86.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="66.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="56.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="51" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="47.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.05">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -3212,7 +3173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.05">
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -3241,7 +3202,7 @@
         <v>993503</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.05">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -3270,7 +3231,7 @@
         <v>993503</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.05">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -3299,7 +3260,7 @@
         <v>993503</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.05">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -3329,33 +3290,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3f5e5cec-56bb-4ca4-8469-5bcbbc5365e6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="79.57142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="111.28571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="60.285714285714285" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="78.28571428571429" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="74.14285714285714" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="57.57142857142857" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="66.28571428571429" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="88.14285714285714" collapsed="true"/>
-    <col min="9" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="79.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="111.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="60.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="78.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="74.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="57.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="66.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="88.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.05">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -3381,7 +3340,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.05">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -3407,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.05">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -3433,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.05">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -3459,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.05">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -3485,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.05">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -3511,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.05">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -3538,34 +3497,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d3f40ae2-e92a-44a2-b510-7b67d542c023}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="52.42857142857143" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="67.71428571428571" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="65.42857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="63.714285714285715" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="40.0" collapsed="true"/>
-    <col min="6" max="7" style="3" width="21.571428571428573" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="3" width="55.42857142857143" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="36.42857142857143" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="3" width="44.714285714285715" collapsed="true"/>
-    <col min="12" max="16384" style="3" width="21.571428571428573" collapsed="true"/>
+    <col min="1" max="1" width="52.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="67.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="63.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="40" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="21.5703125" style="3" collapsed="1"/>
+    <col min="8" max="9" width="55.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="44.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="21.5703125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.05">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -3600,7 +3557,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.05">
+    <row r="2" spans="1:11">
       <c r="A2" s="9" t="s">
         <v>60</v>
       </c>
@@ -3633,7 +3590,7 @@
       </c>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="14.05">
+    <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
@@ -3666,7 +3623,7 @@
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="14.05">
+    <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
@@ -3701,7 +3658,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.05">
+    <row r="5" spans="1:11">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -3713,7 +3670,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="14.05">
+    <row r="6" spans="1:11">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -3726,42 +3683,42 @@
       <c r="J6" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40354208-95a7-41e5-898c-f6e8df345417}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="S1">
-      <selection pane="topLeft" activeCell="V16" sqref="V16"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.424285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="62.42857142857143" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="69.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="46.0" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="13" width="68.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="56.42857142857143" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="13" width="50.857142857142854" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="62.42857142857143" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="13" width="54.285714285714285" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="13" width="48.285714285714285" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="13" width="47.285714285714285" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="13" width="42.285714285714285" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="13" width="20.142857142857142" collapsed="true"/>
-    <col min="16" max="20" customWidth="true" style="13" width="46.142857142857146" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" style="13" width="32.57142857142857" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" style="13" width="53.142857142857146" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="13" width="38.142857142857146" collapsed="true"/>
-    <col min="26" max="16384" style="13" width="21.428571428571427" collapsed="true"/>
+    <col min="1" max="1" width="42.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="62.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="69" style="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46" style="13" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="68" style="13" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="56.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="50.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="62.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="54.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="48.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="47.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="42.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="16" max="20" width="46.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="32.5703125" style="13" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="53.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="38.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="26" max="16384" width="21.42578125" style="13" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.05">
+    <row r="1" spans="1:25" ht="15">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -3838,7 +3795,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.8">
+    <row r="2" spans="1:25">
       <c r="A2" s="12" t="s">
         <v>105</v>
       </c>
@@ -3893,7 +3850,7 @@
       </c>
       <c r="Y2" s="18"/>
     </row>
-    <row r="3" spans="1:25" ht="12.8">
+    <row r="3" spans="1:25">
       <c r="A3" s="12" t="s">
         <v>114</v>
       </c>
@@ -3950,7 +3907,7 @@
       </c>
       <c r="Y3" s="18"/>
     </row>
-    <row r="4" spans="1:25" ht="12.8">
+    <row r="4" spans="1:25">
       <c r="A4" s="12" t="s">
         <v>117</v>
       </c>
@@ -4015,7 +3972,7 @@
       </c>
       <c r="Y4" s="18"/>
     </row>
-    <row r="5" spans="1:25" ht="12.8">
+    <row r="5" spans="1:25">
       <c r="A5" s="12" t="s">
         <v>122</v>
       </c>
@@ -4072,7 +4029,7 @@
       </c>
       <c r="Y5" s="18"/>
     </row>
-    <row r="6" spans="1:25" ht="12.8">
+    <row r="6" spans="1:25">
       <c r="A6" s="12" t="s">
         <v>125</v>
       </c>
@@ -4129,7 +4086,7 @@
       </c>
       <c r="Y6" s="18"/>
     </row>
-    <row r="7" spans="1:25" ht="12.8">
+    <row r="7" spans="1:25">
       <c r="A7" s="12" t="s">
         <v>128</v>
       </c>
@@ -4186,7 +4143,7 @@
       </c>
       <c r="Y7" s="18"/>
     </row>
-    <row r="8" spans="1:25" ht="12.8">
+    <row r="8" spans="1:25">
       <c r="A8" s="12" t="s">
         <v>131</v>
       </c>
@@ -4257,7 +4214,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="12.8">
+    <row r="9" spans="1:25">
       <c r="A9" s="12" t="s">
         <v>139</v>
       </c>
@@ -4290,7 +4247,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="18"/>
     </row>
-    <row r="10" spans="1:25" ht="12.8">
+    <row r="10" spans="1:25">
       <c r="A10" s="12" t="s">
         <v>140</v>
       </c>
@@ -4357,7 +4314,7 @@
       </c>
       <c r="Y10" s="18"/>
     </row>
-    <row r="11" spans="1:25" ht="12.8">
+    <row r="11" spans="1:25">
       <c r="A11" s="12" t="s">
         <v>142</v>
       </c>
@@ -4426,7 +4383,7 @@
       </c>
       <c r="Y11" s="18"/>
     </row>
-    <row r="12" spans="1:25" ht="12.8">
+    <row r="12" spans="1:25">
       <c r="A12" s="12" t="s">
         <v>145</v>
       </c>
@@ -4498,38 +4455,38 @@
       <c r="Y12" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ae20eb1c-647f-4bfc-b26e-dd7391c19518}">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.424285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="39.285714285714285" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="66.71428571428571" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="16.1796875" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="13" width="58.57142857142857" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="13" width="51.42857142857143" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="62.285714285714285" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="13" width="60.285714285714285" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="13" width="42.857142857142854" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="52.857142857142854" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="13" width="51.285714285714285" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="13" width="41.857142857142854" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="13" width="27.714285714285715" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="13" width="34.285714285714285" collapsed="true"/>
-    <col min="15" max="16384" style="13" width="21.428571428571427" collapsed="true"/>
+    <col min="1" max="1" width="39.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="66.7109375" style="13" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="58.5703125" style="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="62.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="60.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="42.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="52.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="51.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="41.85546875" style="13" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27.7109375" style="13" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="34.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="21.42578125" style="13" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.05">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -4573,15 +4530,17 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="12.8">
+    <row r="2" spans="1:14">
       <c r="A2" s="12" t="s">
         <v>161</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="E2" s="15">
         <v>1</v>
       </c>
@@ -4607,15 +4566,17 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="3" spans="1:14" ht="12.8">
+    <row r="3" spans="1:14">
       <c r="A3" s="12" t="s">
         <v>165</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="E3" s="15">
         <v>1</v>
       </c>
@@ -4641,15 +4602,17 @@
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
     </row>
-    <row r="4" spans="1:14" ht="14.1">
-      <c r="A4" s="21" t="s">
-        <v>169</v>
+    <row r="4" spans="1:14">
+      <c r="A4" s="12" t="s">
+        <v>262</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+        <v>263</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="E4" s="15">
         <v>1</v>
       </c>
@@ -4675,15 +4638,17 @@
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
     </row>
-    <row r="5" spans="1:14" ht="14.1">
-      <c r="A5" s="21" t="s">
-        <v>172</v>
+    <row r="5" spans="1:14">
+      <c r="A5" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+        <v>265</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="E5" s="15">
         <v>1</v>
       </c>
@@ -4709,24 +4674,22 @@
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
     </row>
-    <row r="6" spans="1:14" ht="12.8">
+    <row r="6" spans="1:14">
       <c r="A6" s="12" t="s">
-        <v>173</v>
+        <v>266</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>254</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="C6" s="22"/>
       <c r="D6" s="12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E6" s="15">
         <v>1</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>63</v>
@@ -4747,24 +4710,22 @@
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
     </row>
-    <row r="7" spans="1:14" ht="12.8">
+    <row r="7" spans="1:14">
       <c r="A7" s="12" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>175</v>
       </c>
       <c r="E7" s="15">
         <v>1</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>63</v>
@@ -4785,77 +4746,653 @@
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
     </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="15">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+    </row>
+    <row r="19" spans="1:14" ht="14.25">
+      <c r="A19" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+    </row>
+    <row r="20" spans="1:14" ht="14.25">
+      <c r="A20" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+    </row>
+    <row r="21" spans="1:14" ht="14.25">
+      <c r="A21" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="15">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="5.4725" bottom="5.4725" header="5.2756" footer="5.2756"/>
-  <pageSetup orientation="portrait" paperSize="1"/>
+  <pageMargins left="0.7" right="0.7" top="5.4725000000000001" bottom="5.4725000000000001" header="5.2755999999999998" footer="5.2755999999999998"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021ea185-1ac1-4344-9b58-55fe8cb6020b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.284285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="28" width="20.428571428571427" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="28" width="102.85714285714286" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="28" width="77.85714285714286" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="28" width="15.714285714285714" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" style="28" width="90.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="28" width="60.285714285714285" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="28" width="59.714285714285715" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="28" width="57.57142857142857" collapsed="true"/>
-    <col min="11" max="16384" style="13" width="19.285714285714285" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="28" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="102.85546875" style="28" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="77.85546875" style="28" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" style="28" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="90" style="28" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="60.28515625" style="28" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="59.7109375" style="28" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="57.5703125" style="28" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="19.28515625" style="13" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.05">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="26" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.05">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>106</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
@@ -4864,18 +5401,18 @@
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" ht="14.05">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="27">
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>162</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -4884,18 +5421,18 @@
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:10" ht="14.05">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="27">
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>115</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
@@ -4904,18 +5441,18 @@
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" ht="14.05">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="27">
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>118</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
@@ -4924,18 +5461,18 @@
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
     </row>
-    <row r="6" spans="1:10" ht="14.05">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="27">
         <v>5</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
@@ -4944,18 +5481,18 @@
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:10" ht="14.05">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="27">
         <v>6</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>126</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
@@ -4964,18 +5501,18 @@
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" ht="14.05">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="27">
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>129</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
@@ -4984,21 +5521,21 @@
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" ht="14.05">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="27">
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>132</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
@@ -5006,18 +5543,18 @@
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
     </row>
-    <row r="10" spans="1:10" ht="14.05">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="27">
         <v>9</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>138</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
@@ -5026,18 +5563,18 @@
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
     </row>
-    <row r="11" spans="1:10" ht="14.05">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="27">
         <v>10</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>141</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
@@ -5046,18 +5583,18 @@
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
     </row>
-    <row r="12" spans="1:10" ht="14.05">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="27">
         <v>11</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>143</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -5066,18 +5603,18 @@
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" ht="14.05">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="27">
         <v>12</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>146</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -5086,18 +5623,18 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
     </row>
-    <row r="14" spans="1:10" ht="14.05">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="27">
         <v>13</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
@@ -5106,18 +5643,18 @@
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="14.05">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="27">
         <v>14</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
@@ -5126,18 +5663,18 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="14.05">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="27">
         <v>15</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
@@ -5146,18 +5683,18 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
     </row>
-    <row r="17" spans="1:10" ht="14.05">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="27">
         <v>16</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
@@ -5166,18 +5703,18 @@
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
     </row>
-    <row r="18" spans="1:10" ht="14.05">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" s="27">
         <v>17</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
@@ -5186,18 +5723,18 @@
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
     </row>
-    <row r="19" spans="1:10" ht="14.05">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" s="27">
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
@@ -5206,18 +5743,18 @@
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
     </row>
-    <row r="20" spans="1:10" ht="14.05">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" s="27">
         <v>19</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
@@ -5232,8 +5769,8 @@
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7874" right="0.7874" top="1.0835000000000001" bottom="1.0835000000000001" header="0.9445000000000001" footer="0.9445000000000001"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.0835000000000001" bottom="1.0835000000000001" header="0.94450000000000012" footer="0.94450000000000012"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;10Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Commit on 19 May 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="308">
   <si>
     <t>Stage</t>
   </si>
@@ -1007,6 +1007,9 @@
   </si>
   <si>
     <t>DS01_TSA_007</t>
+  </si>
+  <si>
+    <t>TSA_023</t>
   </si>
 </sst>
 </file>
@@ -1026,15 +1029,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
@@ -1046,18 +1060,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF111111"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1171,6 +1174,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF7F7F7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1190,12 +1199,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F7F7F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,7 +1248,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -1277,36 +1280,43 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment/>
       <protection/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -1315,10 +1325,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1326,184 +1341,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="25" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="25" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="25" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="25" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="25" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="25" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="25" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="25" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="25" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="24" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="24" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="32">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
     <cellStyle name="Currency" xfId="16" builtinId="4"/>
@@ -1514,23 +1529,28 @@
     <cellStyle name="Result2" xfId="21"/>
     <cellStyle name="Heading" xfId="22"/>
     <cellStyle name="Heading1" xfId="23"/>
-    <cellStyle name="Excel_5f_5f_5f_20_5f_5f_5f_Built-in_5f_5f_5f_20_5f_5f_5f_Normal" xfId="24"/>
+    <cellStyle name="Excel_5f_20_5f_Built-in_5f_20_5f_Normal" xfId="24"/>
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="25"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="26"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="27"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="28"/>
-    <cellStyle name="Heading_20_1" xfId="29"/>
-    <cellStyle name="Heading1_20_1" xfId="30"/>
-    <cellStyle name="Heading1_5f_20_5f_1" xfId="31"/>
-    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="32"/>
-    <cellStyle name="Heading_5f_20_5f_1" xfId="33"/>
-    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="34"/>
-    <cellStyle name="Result_20_1" xfId="35"/>
-    <cellStyle name="Result2_20_1" xfId="36"/>
-    <cellStyle name="Result2_5f_20_5f_1" xfId="37"/>
-    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="38"/>
-    <cellStyle name="Result_5f_20_5f_1" xfId="39"/>
-    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="40"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="27"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="28"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="29"/>
+    <cellStyle name="Heading_20_1" xfId="30"/>
+    <cellStyle name="Heading1_20_1" xfId="31"/>
+    <cellStyle name="Heading1_5f_20_5f_1" xfId="32"/>
+    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="33"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="34"/>
+    <cellStyle name="Heading_5f_20_5f_1" xfId="35"/>
+    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="36"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="37"/>
+    <cellStyle name="Result_20_1" xfId="38"/>
+    <cellStyle name="Result2_20_1" xfId="39"/>
+    <cellStyle name="Result2_5f_20_5f_1" xfId="40"/>
+    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="41"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="42"/>
+    <cellStyle name="Result_5f_20_5f_1" xfId="43"/>
+    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="44"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="45"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1907,21 +1927,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{a4f6860c-770b-44c2-833a-12478f0aab4b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08eb8634-9a39-46b3-b884-151683353d45}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="60.285714285714285" style="3" customWidth="1"/>
-    <col min="2" max="2" width="73.57142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.285714285714285" style="3" customWidth="1"/>
-    <col min="4" max="4" width="48.285714285714285" style="3" customWidth="1"/>
-    <col min="5" max="5" width="57" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="63.714285714285715" style="3" customWidth="1"/>
+    <col min="2" max="2" width="77.85714285714286" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.57142857142857" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.285714285714285" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -1959,88 +1979,88 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e0ba2961-6163-46a8-bdbc-ad017e8d913b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65e4d25b-9e60-44d0-8e91-f0a00069eff6}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.284285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="16.144285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="19.428571428571427" style="24" customWidth="1"/>
-    <col min="2" max="2" width="41.42857142857143" style="24" customWidth="1"/>
-    <col min="3" max="3" width="46.857142857142854" style="24" customWidth="1"/>
-    <col min="4" max="4" width="18.428571428571427" style="24" customWidth="1"/>
-    <col min="5" max="5" width="49.857142857142854" style="24" customWidth="1"/>
-    <col min="6" max="6" width="50" style="24" customWidth="1"/>
-    <col min="7" max="7" width="53.57142857142857" style="24" customWidth="1"/>
-    <col min="8" max="8" width="64.14285714285714" style="24" customWidth="1"/>
-    <col min="9" max="9" width="53" style="24" customWidth="1"/>
-    <col min="10" max="10" width="55.42857142857143" style="24" customWidth="1"/>
-    <col min="11" max="16384" width="15.285714285714286" style="24"/>
+    <col min="1" max="1" width="20.428571428571427" style="33" customWidth="1"/>
+    <col min="2" max="2" width="43.714285714285715" style="33" customWidth="1"/>
+    <col min="3" max="3" width="49.57142857142857" style="33" customWidth="1"/>
+    <col min="4" max="4" width="19.428571428571427" style="33" customWidth="1"/>
+    <col min="5" max="5" width="52.714285714285715" style="33" customWidth="1"/>
+    <col min="6" max="6" width="52.857142857142854" style="33" customWidth="1"/>
+    <col min="7" max="7" width="56.57142857142857" style="33" customWidth="1"/>
+    <col min="8" max="8" width="67.85714285714286" style="33" customWidth="1"/>
+    <col min="9" max="9" width="56" style="33" customWidth="1"/>
+    <col min="10" max="10" width="58.57142857142857" style="33" customWidth="1"/>
+    <col min="11" max="16384" width="16.142857142857142" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="24" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
-      <c r="A2" s="36">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="14.05">
-      <c r="A3" s="36">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -2049,18 +2069,18 @@
       <c r="C3" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="14.05">
-      <c r="A4" s="36">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2069,18 +2089,18 @@
       <c r="C4" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="36">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -2089,18 +2109,18 @@
       <c r="C5" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="36">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2109,18 +2129,18 @@
       <c r="C6" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="14.05">
-      <c r="A7" s="36">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -2129,18 +2149,18 @@
       <c r="C7" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="14.05">
-      <c r="A8" s="36">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2149,18 +2169,18 @@
       <c r="C8" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="14.05">
-      <c r="A9" s="36">
+      <c r="A9" s="25">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -2169,18 +2189,18 @@
       <c r="C9" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="14.05">
-      <c r="A10" s="36">
+      <c r="A10" s="25">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -2189,18 +2209,18 @@
       <c r="C10" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="14.05">
-      <c r="A11" s="36">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -2209,18 +2229,18 @@
       <c r="C11" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="14.05">
-      <c r="A12" s="36">
+      <c r="A12" s="25">
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2229,18 +2249,18 @@
       <c r="C12" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="14.05">
-      <c r="A13" s="36">
+      <c r="A13" s="25">
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -2249,18 +2269,18 @@
       <c r="C13" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="14.05">
-      <c r="A14" s="36">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2269,18 +2289,18 @@
       <c r="C14" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="14.05">
-      <c r="A15" s="36">
+      <c r="A15" s="25">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -2289,18 +2309,18 @@
       <c r="C15" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="14.05">
-      <c r="A16" s="36">
+      <c r="A16" s="25">
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2309,18 +2329,18 @@
       <c r="C16" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" ht="14.05">
-      <c r="A17" s="36">
+      <c r="A17" s="25">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -2329,131 +2349,131 @@
       <c r="C17" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" ht="14.05">
-      <c r="A18" s="36">
+      <c r="A18" s="25">
         <v>17</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="42" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="14.05">
-      <c r="A19" s="36">
+      <c r="A19" s="25">
         <v>18</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" ht="14.05">
-      <c r="A20" s="36">
+      <c r="A20" s="25">
         <v>19</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10" ht="14.05">
-      <c r="A21" s="36">
+      <c r="A21" s="25">
         <v>20</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="42" t="s">
+      <c r="C21" s="29"/>
+      <c r="D21" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10" ht="14.05">
-      <c r="A22" s="36">
+      <c r="A22" s="25">
         <v>21</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" ht="14.05">
-      <c r="A23" s="36">
+      <c r="A23" s="25">
         <v>22</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2461,46 +2481,46 @@
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="3.7016" bottom="3.7016" header="3.5046999999999997" footer="3.5046999999999997"/>
+  <pageMargins left="0.7" right="0.7" top="3.9969" bottom="3.9969" header="3.8" footer="3.8"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48528f39-0968-4e0d-a0e3-439123bba0d6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e9860819-c807-4222-8e8d-5c6776c97ae3}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.424285714285714" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="15.284285714285714" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="51" style="24" customWidth="1"/>
-    <col min="2" max="2" width="53.857142857142854" style="24" customWidth="1"/>
-    <col min="3" max="9" width="41" style="24" customWidth="1"/>
-    <col min="10" max="10" width="45" style="24" customWidth="1"/>
-    <col min="11" max="11" width="51.42857142857143" style="24" customWidth="1"/>
-    <col min="12" max="12" width="50.57142857142857" style="24" customWidth="1"/>
-    <col min="13" max="13" width="40" style="24" customWidth="1"/>
-    <col min="14" max="14" width="39.285714285714285" style="24" customWidth="1"/>
-    <col min="15" max="15" width="45.57142857142857" style="24" customWidth="1"/>
-    <col min="16" max="16" width="50" style="24" customWidth="1"/>
-    <col min="17" max="17" width="41.42857142857143" style="24" customWidth="1"/>
-    <col min="18" max="18" width="33" style="24" customWidth="1"/>
-    <col min="19" max="19" width="37.42857142857143" style="24" customWidth="1"/>
-    <col min="20" max="20" width="54.42857142857143" style="24" customWidth="1"/>
-    <col min="21" max="21" width="53.857142857142854" style="24" customWidth="1"/>
-    <col min="22" max="22" width="53.42857142857143" style="24" customWidth="1"/>
-    <col min="23" max="23" width="53.57142857142857" style="24" customWidth="1"/>
-    <col min="24" max="24" width="51.285714285714285" style="24" customWidth="1"/>
-    <col min="25" max="25" width="38.857142857142854" style="24" customWidth="1"/>
-    <col min="26" max="26" width="48.714285714285715" style="24" customWidth="1"/>
-    <col min="27" max="27" width="30.857142857142858" style="24" customWidth="1"/>
-    <col min="28" max="28" width="44.714285714285715" style="24" customWidth="1"/>
-    <col min="29" max="29" width="33.57142857142857" style="24" customWidth="1"/>
-    <col min="30" max="30" width="28.142857142857142" style="24" customWidth="1"/>
-    <col min="31" max="16384" width="14.428571428571429" style="24"/>
+    <col min="1" max="1" width="53.857142857142854" style="33" customWidth="1"/>
+    <col min="2" max="2" width="57" style="33" customWidth="1"/>
+    <col min="3" max="9" width="43.285714285714285" style="33" customWidth="1"/>
+    <col min="10" max="10" width="47.57142857142857" style="33" customWidth="1"/>
+    <col min="11" max="11" width="54.42857142857143" style="33" customWidth="1"/>
+    <col min="12" max="12" width="53.42857142857143" style="33" customWidth="1"/>
+    <col min="13" max="13" width="42.285714285714285" style="33" customWidth="1"/>
+    <col min="14" max="14" width="41.42857142857143" style="33" customWidth="1"/>
+    <col min="15" max="15" width="48.142857142857146" style="33" customWidth="1"/>
+    <col min="16" max="16" width="52.857142857142854" style="33" customWidth="1"/>
+    <col min="17" max="17" width="43.714285714285715" style="33" customWidth="1"/>
+    <col min="18" max="18" width="34.857142857142854" style="33" customWidth="1"/>
+    <col min="19" max="19" width="39.57142857142857" style="33" customWidth="1"/>
+    <col min="20" max="20" width="57.57142857142857" style="33" customWidth="1"/>
+    <col min="21" max="21" width="57" style="33" customWidth="1"/>
+    <col min="22" max="22" width="56.42857142857143" style="33" customWidth="1"/>
+    <col min="23" max="23" width="56.57142857142857" style="33" customWidth="1"/>
+    <col min="24" max="24" width="54.142857142857146" style="33" customWidth="1"/>
+    <col min="25" max="25" width="41" style="33" customWidth="1"/>
+    <col min="26" max="26" width="51.42857142857143" style="33" customWidth="1"/>
+    <col min="27" max="27" width="32.57142857142857" style="33" customWidth="1"/>
+    <col min="28" max="28" width="47.285714285714285" style="33" customWidth="1"/>
+    <col min="29" max="29" width="35.42857142857143" style="33" customWidth="1"/>
+    <col min="30" max="30" width="29.714285714285715" style="33" customWidth="1"/>
+    <col min="31" max="16384" width="15.285714285714286" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.05">
@@ -3376,7 +3396,7 @@
       <c r="AD14" s="18"/>
     </row>
     <row r="15" spans="1:30" ht="12.8">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="35" t="s">
         <v>268</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -3426,7 +3446,7 @@
       <c r="AD15" s="18"/>
     </row>
     <row r="16" spans="1:30" ht="12.8">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="35" t="s">
         <v>272</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -3476,33 +3496,33 @@
       <c r="AD16" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="3.4063000000000003" bottom="3.4063000000000003" header="3.2094" footer="3.2094"/>
+  <pageMargins left="0.7" right="0.7" top="3.7016" bottom="3.7016" header="3.5046999999999997" footer="3.5046999999999997"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e0c143cb-ce3a-442c-9077-2c9b8f977591}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75d71288-c06c-4cb0-abf3-95a5c20ca8b5}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.714285714285714" defaultRowHeight="21.55"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="20.285714285714285" style="28" customWidth="1"/>
-    <col min="2" max="2" width="23" style="28" customWidth="1"/>
-    <col min="3" max="3" width="14.857142857142858" style="28" customWidth="1"/>
-    <col min="4" max="4" width="32.142857142857146" style="28" customWidth="1"/>
-    <col min="5" max="5" width="34.714285714285715" style="28" customWidth="1"/>
-    <col min="6" max="6" width="31.714285714285715" style="28" customWidth="1"/>
-    <col min="7" max="7" width="38.42857142857143" style="28" customWidth="1"/>
-    <col min="8" max="8" width="27.714285714285715" style="28" customWidth="1"/>
-    <col min="9" max="9" width="29" style="28" customWidth="1"/>
-    <col min="10" max="10" width="29.285714285714285" style="28" customWidth="1"/>
-    <col min="11" max="11" width="16.571428571428573" style="28" customWidth="1"/>
-    <col min="12" max="16384" width="13.714285714285714" style="28"/>
+    <col min="1" max="1" width="21.428571428571427" style="38" customWidth="1"/>
+    <col min="2" max="2" width="24.285714285714285" style="38" customWidth="1"/>
+    <col min="3" max="3" width="15.714285714285714" style="38" customWidth="1"/>
+    <col min="4" max="4" width="34" style="38" customWidth="1"/>
+    <col min="5" max="5" width="36.714285714285715" style="38" customWidth="1"/>
+    <col min="6" max="6" width="33.42857142857143" style="38" customWidth="1"/>
+    <col min="7" max="7" width="40.57142857142857" style="38" customWidth="1"/>
+    <col min="8" max="8" width="29.285714285714285" style="38" customWidth="1"/>
+    <col min="9" max="9" width="30.571428571428573" style="38" customWidth="1"/>
+    <col min="10" max="10" width="30.857142857142858" style="38" customWidth="1"/>
+    <col min="11" max="11" width="17.428571428571427" style="38" customWidth="1"/>
+    <col min="12" max="16384" width="14.571428571428571" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -3512,270 +3532,270 @@
       <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="43" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="12.8">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="40">
         <v>7402</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="40">
         <v>2</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="40">
         <v>2</v>
       </c>
-      <c r="K2" s="34"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11" ht="12.8">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="40">
         <v>7402</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="34"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11" ht="12.8">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="37" t="s">
         <v>290</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="40" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="40">
         <v>7402</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="40">
         <v>2</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="40">
         <v>2</v>
       </c>
-      <c r="K4" s="34"/>
+      <c r="K4" s="44"/>
     </row>
     <row r="5" spans="1:11" ht="12.8">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="30">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="40">
         <v>7402</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="34"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:11" ht="25.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="40">
         <v>8795</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="34"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="44"/>
     </row>
     <row r="7" spans="1:11" ht="25.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="40">
         <v>8796</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="34"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="44"/>
     </row>
     <row r="8" spans="1:11" ht="17.85" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="40">
         <v>8797</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="34"/>
-    </row>
-    <row r="9" spans="1:11" ht="21.55">
-      <c r="A9" s="26" t="s">
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="44"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.3">
+      <c r="A9" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="40">
         <v>8798</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="34"/>
-    </row>
-    <row r="10" spans="1:11" ht="21.55">
-      <c r="A10" s="26" t="s">
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="44"/>
+    </row>
+    <row r="10" spans="1:11" ht="12.8">
+      <c r="A10" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="34">
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="44">
         <v>7402</v>
       </c>
     </row>
@@ -3790,195 +3810,207 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{f09d6312-0b98-4c69-afb5-e16781eba163}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336f71c6-9cab-4e65-8302-16fe22062728}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.714285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="13.428571428571429" style="28" customWidth="1"/>
-    <col min="2" max="2" width="28.857142857142858" style="28" customWidth="1"/>
-    <col min="3" max="3" width="27.285714285714285" style="28" customWidth="1"/>
-    <col min="4" max="4" width="16.571428571428573" style="28" customWidth="1"/>
-    <col min="5" max="5" width="36.142857142857146" style="28" customWidth="1"/>
-    <col min="6" max="6" width="31.142857142857142" style="28" customWidth="1"/>
-    <col min="7" max="7" width="32.285714285714285" style="28" customWidth="1"/>
-    <col min="8" max="8" width="31.571428571428573" style="28" customWidth="1"/>
-    <col min="9" max="9" width="31.428571428571427" style="28" customWidth="1"/>
-    <col min="10" max="10" width="31.285714285714285" style="28" customWidth="1"/>
-    <col min="11" max="16384" width="13.714285714285714" style="28"/>
+    <col min="1" max="1" width="14.142857142857142" style="38" customWidth="1"/>
+    <col min="2" max="2" width="30.428571428571427" style="38" customWidth="1"/>
+    <col min="3" max="3" width="28.857142857142858" style="38" customWidth="1"/>
+    <col min="4" max="4" width="17.428571428571427" style="38" customWidth="1"/>
+    <col min="5" max="5" width="38.142857142857146" style="38" customWidth="1"/>
+    <col min="6" max="6" width="32.857142857142854" style="38" customWidth="1"/>
+    <col min="7" max="7" width="34.142857142857146" style="38" customWidth="1"/>
+    <col min="8" max="8" width="33.285714285714285" style="38" customWidth="1"/>
+    <col min="9" max="9" width="33.142857142857146" style="38" customWidth="1"/>
+    <col min="10" max="10" width="33" style="38" customWidth="1"/>
+    <col min="11" max="16384" width="14.571428571428571" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="24" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.05">
-      <c r="A2" s="27">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="37" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.05">
-      <c r="A3" s="27">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.05">
-      <c r="A4" s="27">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="37" t="s">
         <v>290</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="37" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.05">
-      <c r="A5" s="27">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.05">
-      <c r="A6" s="27">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.05">
-      <c r="A7" s="27">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.05">
-      <c r="A8" s="27">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.05">
-      <c r="A9" s="27">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="31" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.05">
-      <c r="A10" s="27">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="36" t="s">
         <v>306</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.05">
+      <c r="A11" s="37">
+        <v>9</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="31" t="s">
         <v>224</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3992,21 +4024,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{dcbc99ef-5a5d-49f8-93ea-cc459dd55476}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9f08c860-473f-424a-a6c4-53e8ee629f2d}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="C1">
       <selection pane="topLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="50" style="3" customWidth="1"/>
-    <col min="2" max="2" width="60.714285714285715" style="3" customWidth="1"/>
-    <col min="3" max="3" width="58.57142857142857" style="3" customWidth="1"/>
-    <col min="4" max="4" width="74.14285714285714" style="3" customWidth="1"/>
-    <col min="5" max="5" width="93.14285714285714" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="52.857142857142854" style="3" customWidth="1"/>
+    <col min="2" max="2" width="64.14285714285714" style="3" customWidth="1"/>
+    <col min="3" max="3" width="61.857142857142854" style="3" customWidth="1"/>
+    <col min="4" max="4" width="78.42857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="98.42857142857143" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -4061,25 +4093,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ff523f1-d27b-4316-b1c3-2d4a2eb40dd3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41391527-2827-4154-be93-f6c9d9b1329c}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="25.571428571428573" style="3"/>
-    <col min="2" max="2" width="89.57142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="79.57142857142857" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="27" style="3"/>
+    <col min="2" max="2" width="94.71428571428571" style="3" customWidth="1"/>
+    <col min="3" max="3" width="84.14285714285714" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.05">
@@ -4105,30 +4137,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54ddeff9-9b18-4006-897c-7604e19c731b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30d8b873-4f3b-443d-8f12-45bfca2224d0}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="68" style="3" customWidth="1"/>
-    <col min="2" max="2" width="102.14285714285714" style="3" customWidth="1"/>
-    <col min="3" max="3" width="78.85714285714286" style="3" customWidth="1"/>
-    <col min="4" max="4" width="69.71428571428571" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.285714285714285" style="3" customWidth="1"/>
-    <col min="6" max="6" width="66.71428571428571" style="3" customWidth="1"/>
-    <col min="7" max="8" width="60.285714285714285" style="3" customWidth="1"/>
-    <col min="9" max="9" width="56.42857142857143" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="71.85714285714286" style="3" customWidth="1"/>
+    <col min="2" max="2" width="108" style="3" customWidth="1"/>
+    <col min="3" max="3" width="83.42857142857143" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73.71428571428571" style="3" customWidth="1"/>
+    <col min="5" max="5" width="63.714285714285715" style="3" customWidth="1"/>
+    <col min="6" max="6" width="70.57142857142857" style="3" customWidth="1"/>
+    <col min="7" max="8" width="63.714285714285715" style="3" customWidth="1"/>
+    <col min="9" max="9" width="59.714285714285715" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.05">
@@ -4277,30 +4309,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b45a835a-36e6-42b6-9b3e-bdffc6d57fae}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5a994e50-2ed2-4850-98c1-54f0265d9ced}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="94.14285714285714" style="3" customWidth="1"/>
-    <col min="2" max="2" width="131.71428571428572" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.14285714285714" style="3" customWidth="1"/>
-    <col min="4" max="4" width="92.42857142857143" style="3" customWidth="1"/>
-    <col min="5" max="5" width="87.57142857142857" style="3" customWidth="1"/>
-    <col min="6" max="6" width="68" style="3" customWidth="1"/>
-    <col min="7" max="7" width="78.42857142857143" style="3" customWidth="1"/>
-    <col min="8" max="8" width="104.14285714285714" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="99.57142857142857" style="3" customWidth="1"/>
+    <col min="2" max="2" width="139.28571428571428" style="3" customWidth="1"/>
+    <col min="3" max="3" width="75.28571428571429" style="3" customWidth="1"/>
+    <col min="4" max="4" width="97.71428571428571" style="3" customWidth="1"/>
+    <col min="5" max="5" width="92.57142857142857" style="3" customWidth="1"/>
+    <col min="6" max="6" width="71.85714285714286" style="3" customWidth="1"/>
+    <col min="7" max="7" width="82.85714285714286" style="3" customWidth="1"/>
+    <col min="8" max="8" width="110.14285714285714" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.05">
@@ -4486,31 +4518,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3636b7fa-b064-4be2-a67a-a0a5ddbfc0f5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d6dac21d-1c4b-443f-ae7a-40cb8690d10a}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.574285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="61.857142857142854" style="3" customWidth="1"/>
-    <col min="2" max="2" width="80" style="3" customWidth="1"/>
-    <col min="3" max="3" width="77.28571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="75.28571428571429" style="3" customWidth="1"/>
-    <col min="5" max="5" width="47.285714285714285" style="3" customWidth="1"/>
-    <col min="6" max="7" width="25.571428571428573" style="3"/>
-    <col min="8" max="9" width="65.42857142857143" style="3" customWidth="1"/>
-    <col min="10" max="10" width="42.857142857142854" style="3" customWidth="1"/>
-    <col min="11" max="11" width="52.857142857142854" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="25.571428571428573" style="3"/>
+    <col min="1" max="1" width="65.42857142857143" style="3" customWidth="1"/>
+    <col min="2" max="2" width="84.57142857142857" style="3" customWidth="1"/>
+    <col min="3" max="3" width="81.71428571428571" style="3" customWidth="1"/>
+    <col min="4" max="4" width="79.57142857142857" style="3" customWidth="1"/>
+    <col min="5" max="5" width="50" style="3" customWidth="1"/>
+    <col min="6" max="7" width="27" style="3"/>
+    <col min="8" max="9" width="69.14285714285714" style="3" customWidth="1"/>
+    <col min="10" max="10" width="45.285714285714285" style="3" customWidth="1"/>
+    <col min="11" max="11" width="55.857142857142854" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="27" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -4549,10 +4581,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.05">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4579,13 +4611,13 @@
       <c r="J2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="8"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="14.05">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -4612,13 +4644,13 @@
       <c r="J3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="8"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" ht="14.05">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -4645,68 +4677,68 @@
       <c r="J4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0d5f2760-aa24-435a-bbc3-f45e772d976a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69342407-d2b7-4fec-8e82-ca1e0d471fb8}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="S1">
       <selection pane="topLeft" activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.424285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="26.854285714285716" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="50" style="13" customWidth="1"/>
-    <col min="2" max="2" width="73.71428571428571" style="13" customWidth="1"/>
-    <col min="3" max="3" width="81.57142857142857" style="13" customWidth="1"/>
-    <col min="4" max="4" width="54.142857142857146" style="13" customWidth="1"/>
-    <col min="5" max="6" width="80.42857142857143" style="13" customWidth="1"/>
-    <col min="7" max="7" width="66.71428571428571" style="13" customWidth="1"/>
-    <col min="8" max="9" width="60" style="13" customWidth="1"/>
-    <col min="10" max="10" width="73.71428571428571" style="13" customWidth="1"/>
-    <col min="11" max="11" width="64.14285714285714" style="13" customWidth="1"/>
-    <col min="12" max="12" width="57" style="13" customWidth="1"/>
-    <col min="13" max="13" width="55.857142857142854" style="13" customWidth="1"/>
-    <col min="14" max="14" width="50" style="13" customWidth="1"/>
-    <col min="15" max="15" width="23.714285714285715" style="13" customWidth="1"/>
-    <col min="16" max="20" width="54.42857142857143" style="13" customWidth="1"/>
-    <col min="21" max="22" width="38.42857142857143" style="13" customWidth="1"/>
-    <col min="23" max="24" width="62.714285714285715" style="13" customWidth="1"/>
-    <col min="25" max="25" width="45" style="13" customWidth="1"/>
-    <col min="26" max="16384" width="25.428571428571427" style="13"/>
+    <col min="1" max="1" width="52.857142857142854" style="13" customWidth="1"/>
+    <col min="2" max="2" width="78" style="13" customWidth="1"/>
+    <col min="3" max="3" width="86.28571428571429" style="13" customWidth="1"/>
+    <col min="4" max="4" width="57.285714285714285" style="13" customWidth="1"/>
+    <col min="5" max="6" width="85" style="13" customWidth="1"/>
+    <col min="7" max="7" width="70.57142857142857" style="13" customWidth="1"/>
+    <col min="8" max="9" width="63.42857142857143" style="13" customWidth="1"/>
+    <col min="10" max="10" width="78" style="13" customWidth="1"/>
+    <col min="11" max="11" width="67.85714285714286" style="13" customWidth="1"/>
+    <col min="12" max="12" width="60.285714285714285" style="13" customWidth="1"/>
+    <col min="13" max="13" width="59" style="13" customWidth="1"/>
+    <col min="14" max="14" width="52.857142857142854" style="13" customWidth="1"/>
+    <col min="15" max="15" width="25" style="13" customWidth="1"/>
+    <col min="16" max="20" width="57.57142857142857" style="13" customWidth="1"/>
+    <col min="21" max="22" width="40.57142857142857" style="13" customWidth="1"/>
+    <col min="23" max="24" width="66.28571428571429" style="13" customWidth="1"/>
+    <col min="25" max="25" width="47.57142857142857" style="13" customWidth="1"/>
+    <col min="26" max="16384" width="26.857142857142858" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.05">
@@ -5446,35 +5478,35 @@
       <c r="Y12" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e7a5b368-cd23-4ab8-a6e9-284b67e804f1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4c1baa5d-7fb4-482f-8342-d55018f6955b}">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.424285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="26.854285714285716" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="46.142857142857146" style="13" customWidth="1"/>
-    <col min="2" max="2" width="78.85714285714286" style="13" customWidth="1"/>
-    <col min="3" max="3" width="18.857142857142858" style="13" customWidth="1"/>
-    <col min="4" max="5" width="69.14285714285714" style="13" customWidth="1"/>
-    <col min="6" max="6" width="60.714285714285715" style="13" customWidth="1"/>
-    <col min="7" max="7" width="73.57142857142857" style="13" customWidth="1"/>
-    <col min="8" max="8" width="71.14285714285714" style="13" customWidth="1"/>
-    <col min="9" max="9" width="50.57142857142857" style="13" customWidth="1"/>
-    <col min="10" max="10" width="62.42857142857143" style="13" customWidth="1"/>
-    <col min="11" max="11" width="60.57142857142857" style="13" customWidth="1"/>
-    <col min="12" max="12" width="49.57142857142857" style="13" customWidth="1"/>
-    <col min="13" max="13" width="32.57142857142857" style="13" customWidth="1"/>
-    <col min="14" max="14" width="40.285714285714285" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="25.428571428571427" style="13"/>
+    <col min="1" max="1" width="48.714285714285715" style="13" customWidth="1"/>
+    <col min="2" max="2" width="83.42857142857143" style="13" customWidth="1"/>
+    <col min="3" max="3" width="19.857142857142858" style="13" customWidth="1"/>
+    <col min="4" max="5" width="73.14285714285714" style="13" customWidth="1"/>
+    <col min="6" max="6" width="64.14285714285714" style="13" customWidth="1"/>
+    <col min="7" max="7" width="77.85714285714286" style="13" customWidth="1"/>
+    <col min="8" max="8" width="75.28571428571429" style="13" customWidth="1"/>
+    <col min="9" max="9" width="53.42857142857143" style="13" customWidth="1"/>
+    <col min="10" max="10" width="66" style="13" customWidth="1"/>
+    <col min="11" max="11" width="64" style="13" customWidth="1"/>
+    <col min="12" max="12" width="52.42857142857143" style="13" customWidth="1"/>
+    <col min="13" max="13" width="34.42857142857143" style="13" customWidth="1"/>
+    <col min="14" max="14" width="42.57142857142857" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="26.857142857142858" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.05">
@@ -6314,445 +6346,445 @@
       <c r="N23" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.3579" bottom="6.3579" header="6.161" footer="6.161"/>
+  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{cb76a99d-17b4-41fc-9591-008af74c922f}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1beb3ac7-bc64-4d3b-8d44-2c890b47a65a}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.854285714285716" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="24.144285714285715" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="24" style="37" customWidth="1"/>
-    <col min="2" max="2" width="121.57142857142857" style="37" customWidth="1"/>
-    <col min="3" max="3" width="92" style="37" customWidth="1"/>
-    <col min="4" max="4" width="18.428571428571427" style="37" customWidth="1"/>
-    <col min="5" max="7" width="106.28571428571429" style="37" customWidth="1"/>
-    <col min="8" max="8" width="71.14285714285714" style="37" customWidth="1"/>
-    <col min="9" max="9" width="70.57142857142857" style="37" customWidth="1"/>
-    <col min="10" max="10" width="68" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="22.857142857142858" style="13"/>
+    <col min="1" max="1" width="25.285714285714285" style="26" customWidth="1"/>
+    <col min="2" max="2" width="128.57142857142858" style="26" customWidth="1"/>
+    <col min="3" max="3" width="97.28571428571429" style="26" customWidth="1"/>
+    <col min="4" max="4" width="19.428571428571427" style="26" customWidth="1"/>
+    <col min="5" max="7" width="112.42857142857143" style="26" customWidth="1"/>
+    <col min="8" max="8" width="75.28571428571429" style="26" customWidth="1"/>
+    <col min="9" max="9" width="74.57142857142857" style="26" customWidth="1"/>
+    <col min="10" max="10" width="71.85714285714286" style="26" customWidth="1"/>
+    <col min="11" max="16384" width="24.142857142857142" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="24" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.05">
-      <c r="A2" s="36">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="14.05">
-      <c r="A3" s="36">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="14.05">
-      <c r="A4" s="36">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="14.05">
-      <c r="A5" s="36">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="14.05">
-      <c r="A6" s="36">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="14.05">
-      <c r="A7" s="36">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="14.05">
-      <c r="A8" s="36">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="14.05">
-      <c r="A9" s="36">
+      <c r="A9" s="25">
         <v>8</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="14.05">
-      <c r="A10" s="36">
+      <c r="A10" s="25">
         <v>9</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="14.05">
-      <c r="A11" s="36">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="14.05">
-      <c r="A12" s="36">
+      <c r="A12" s="25">
         <v>11</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="14.05">
-      <c r="A13" s="36">
+      <c r="A13" s="25">
         <v>12</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="14.05">
-      <c r="A14" s="36">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="14.05">
-      <c r="A15" s="36">
+      <c r="A15" s="25">
         <v>14</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="14.05">
-      <c r="A16" s="36">
+      <c r="A16" s="25">
         <v>15</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" ht="14.05">
-      <c r="A17" s="36">
+      <c r="A17" s="25">
         <v>16</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" ht="14.05">
-      <c r="A18" s="36">
+      <c r="A18" s="25">
         <v>17</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="14.05">
-      <c r="A19" s="36">
+      <c r="A19" s="25">
         <v>18</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" ht="14.05">
-      <c r="A20" s="36">
+      <c r="A20" s="25">
         <v>19</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
commit on 22 may 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="CSM_Login" sheetId="1" r:id="rId3"/>
@@ -20,6 +20,8 @@
     <sheet name="CSM_ChargeWaiverTestData" sheetId="11" r:id="rId13"/>
     <sheet name="TrasactionOnStaffAccountTestDat" sheetId="12" r:id="rId14"/>
     <sheet name="TransactionOnStaffAccount_Execu" sheetId="13" r:id="rId15"/>
+    <sheet name="TransactionTestData" sheetId="14" r:id="rId16"/>
+    <sheet name="Transaction_ExecutionTracker" sheetId="15" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="333">
   <si>
     <t>Stage</t>
   </si>
@@ -1010,6 +1012,81 @@
   </si>
   <si>
     <t>TSA_023</t>
+  </si>
+  <si>
+    <t>System Date</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Other Teller Transaction Number</t>
+  </si>
+  <si>
+    <t>Own Teller Transaction number</t>
+  </si>
+  <si>
+    <t>Current Date Transaction number</t>
+  </si>
+  <si>
+    <t>Past transaction number</t>
+  </si>
+  <si>
+    <t>TRS_001</t>
+  </si>
+  <si>
+    <t>DS01_TRS_001</t>
+  </si>
+  <si>
+    <t>22/05/2023</t>
+  </si>
+  <si>
+    <t>TRS_002</t>
+  </si>
+  <si>
+    <t>DS01_TRS_002</t>
+  </si>
+  <si>
+    <t>TRS_003</t>
+  </si>
+  <si>
+    <t>DS01_TRS_003</t>
+  </si>
+  <si>
+    <t>TRS_004</t>
+  </si>
+  <si>
+    <t>DS01_TRS_004</t>
+  </si>
+  <si>
+    <t>TRS_005</t>
+  </si>
+  <si>
+    <t>DS01_TRS_005</t>
+  </si>
+  <si>
+    <t>TRS_006</t>
+  </si>
+  <si>
+    <t>DS01_TRS_006</t>
+  </si>
+  <si>
+    <t>TRS_007</t>
+  </si>
+  <si>
+    <t>DS01_TRS_007</t>
+  </si>
+  <si>
+    <t>TRS_001_01</t>
+  </si>
+  <si>
+    <t>DS01_TRS_001_01</t>
+  </si>
+  <si>
+    <t>TRS_002_01</t>
+  </si>
+  <si>
+    <t>DS01_TRS_002_01</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1202,6 +1279,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1248,7 +1337,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -1304,6 +1393,18 @@
       <alignment/>
       <protection/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1319,6 +1420,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1328,144 +1441,184 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="28" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1473,11 +1626,27 @@
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="28" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="28" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
@@ -1493,32 +1662,40 @@
       <alignment/>
       <protection/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="24" applyFont="1" applyFill="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="24" applyNumberFormat="1" applyFont="1">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="24" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="26" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="26" applyFill="1" applyBorder="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="24" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="24" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="24" applyFont="1" applyFill="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
     <cellStyle name="Currency" xfId="16" builtinId="4"/>
@@ -1533,24 +1710,43 @@
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="25"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="26"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="27"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="28"/>
-    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="29"/>
-    <cellStyle name="Heading_20_1" xfId="30"/>
-    <cellStyle name="Heading1_20_1" xfId="31"/>
-    <cellStyle name="Heading1_5f_20_5f_1" xfId="32"/>
-    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="33"/>
-    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="34"/>
-    <cellStyle name="Heading_5f_20_5f_1" xfId="35"/>
-    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="36"/>
-    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="37"/>
-    <cellStyle name="Result_20_1" xfId="38"/>
-    <cellStyle name="Result2_20_1" xfId="39"/>
-    <cellStyle name="Result2_5f_20_5f_1" xfId="40"/>
-    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="41"/>
-    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="42"/>
-    <cellStyle name="Result_5f_20_5f_1" xfId="43"/>
-    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="44"/>
-    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="45"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="28"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="29"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="30"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Built-in_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_Normal" xfId="31"/>
+    <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="32"/>
+    <cellStyle name="Heading_20_1" xfId="33"/>
+    <cellStyle name="Heading1_20_1" xfId="34"/>
+    <cellStyle name="Heading1_5f_20_5f_1" xfId="35"/>
+    <cellStyle name="Heading1_5f_5f_5f_20_5f_5f_5f_1" xfId="36"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="37"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="38"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="39"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="40"/>
+    <cellStyle name="Heading1_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="41"/>
+    <cellStyle name="Heading_5f_20_5f_1" xfId="42"/>
+    <cellStyle name="Heading_5f_5f_5f_20_5f_5f_5f_1" xfId="43"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="44"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="45"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="46"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="47"/>
+    <cellStyle name="Heading_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="48"/>
+    <cellStyle name="Result_20_1" xfId="49"/>
+    <cellStyle name="Result2_20_1" xfId="50"/>
+    <cellStyle name="Result2_5f_20_5f_1" xfId="51"/>
+    <cellStyle name="Result2_5f_5f_5f_20_5f_5f_5f_1" xfId="52"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="53"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="54"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="55"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="56"/>
+    <cellStyle name="Result2_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="57"/>
+    <cellStyle name="Result_5f_20_5f_1" xfId="58"/>
+    <cellStyle name="Result_5f_5f_5f_20_5f_5f_5f_1" xfId="59"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_1" xfId="60"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="61"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="62"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="63"/>
+    <cellStyle name="Result_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_20_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_1" xfId="64"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1927,21 +2123,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08eb8634-9a39-46b3-b884-151683353d45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8acfda1e-4282-42d7-8d8e-4693445906b4}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="63.714285714285715" style="3" customWidth="1"/>
-    <col min="2" max="2" width="77.85714285714286" style="3" customWidth="1"/>
-    <col min="3" max="3" width="60.57142857142857" style="3" customWidth="1"/>
-    <col min="4" max="4" width="51" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.285714285714285" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="79.57142857142857" style="3" customWidth="1"/>
+    <col min="2" max="2" width="97.28571428571429" style="3" customWidth="1"/>
+    <col min="3" max="3" width="75.71428571428571" style="3" customWidth="1"/>
+    <col min="4" max="4" width="63.714285714285715" style="3" customWidth="1"/>
+    <col min="5" max="5" width="75.28571428571429" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -1979,32 +2175,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65e4d25b-9e60-44d0-8e91-f0a00069eff6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ce51eee-c2bf-4dc4-a6e6-7b33274005e6}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.144285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="20.284285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="20.428571428571427" style="33" customWidth="1"/>
-    <col min="2" max="2" width="43.714285714285715" style="33" customWidth="1"/>
-    <col min="3" max="3" width="49.57142857142857" style="33" customWidth="1"/>
-    <col min="4" max="4" width="19.428571428571427" style="33" customWidth="1"/>
-    <col min="5" max="5" width="52.714285714285715" style="33" customWidth="1"/>
-    <col min="6" max="6" width="52.857142857142854" style="33" customWidth="1"/>
-    <col min="7" max="7" width="56.57142857142857" style="33" customWidth="1"/>
-    <col min="8" max="8" width="67.85714285714286" style="33" customWidth="1"/>
-    <col min="9" max="9" width="56" style="33" customWidth="1"/>
-    <col min="10" max="10" width="58.57142857142857" style="33" customWidth="1"/>
-    <col min="11" max="16384" width="16.142857142857142" style="33"/>
+    <col min="1" max="1" width="25.285714285714285" style="33" customWidth="1"/>
+    <col min="2" max="2" width="54.42857142857143" style="33" customWidth="1"/>
+    <col min="3" max="3" width="61.857142857142854" style="33" customWidth="1"/>
+    <col min="4" max="4" width="24" style="33" customWidth="1"/>
+    <col min="5" max="5" width="65.85714285714286" style="33" customWidth="1"/>
+    <col min="6" max="6" width="66" style="33" customWidth="1"/>
+    <col min="7" max="7" width="70.71428571428571" style="33" customWidth="1"/>
+    <col min="8" max="8" width="84.71428571428571" style="33" customWidth="1"/>
+    <col min="9" max="9" width="70" style="33" customWidth="1"/>
+    <col min="10" max="10" width="73.14285714285714" style="33" customWidth="1"/>
+    <col min="11" max="16384" width="20.285714285714285" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
@@ -2481,46 +2677,46 @@
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="3.9969" bottom="3.9969" header="3.8" footer="3.8"/>
+  <pageMargins left="0.7" right="0.7" top="5.1772" bottom="5.1772" header="4.9803" footer="4.9803"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e9860819-c807-4222-8e8d-5c6776c97ae3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9139658b-feff-4bae-9d9e-49cd5413ccfb}">
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.284285714285714" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="19.144285714285715" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="53.857142857142854" style="33" customWidth="1"/>
-    <col min="2" max="2" width="57" style="33" customWidth="1"/>
-    <col min="3" max="9" width="43.285714285714285" style="33" customWidth="1"/>
-    <col min="10" max="10" width="47.57142857142857" style="33" customWidth="1"/>
-    <col min="11" max="11" width="54.42857142857143" style="33" customWidth="1"/>
-    <col min="12" max="12" width="53.42857142857143" style="33" customWidth="1"/>
-    <col min="13" max="13" width="42.285714285714285" style="33" customWidth="1"/>
-    <col min="14" max="14" width="41.42857142857143" style="33" customWidth="1"/>
-    <col min="15" max="15" width="48.142857142857146" style="33" customWidth="1"/>
-    <col min="16" max="16" width="52.857142857142854" style="33" customWidth="1"/>
-    <col min="17" max="17" width="43.714285714285715" style="33" customWidth="1"/>
-    <col min="18" max="18" width="34.857142857142854" style="33" customWidth="1"/>
-    <col min="19" max="19" width="39.57142857142857" style="33" customWidth="1"/>
-    <col min="20" max="20" width="57.57142857142857" style="33" customWidth="1"/>
-    <col min="21" max="21" width="57" style="33" customWidth="1"/>
-    <col min="22" max="22" width="56.42857142857143" style="33" customWidth="1"/>
-    <col min="23" max="23" width="56.57142857142857" style="33" customWidth="1"/>
-    <col min="24" max="24" width="54.142857142857146" style="33" customWidth="1"/>
-    <col min="25" max="25" width="41" style="33" customWidth="1"/>
-    <col min="26" max="26" width="51.42857142857143" style="33" customWidth="1"/>
-    <col min="27" max="27" width="32.57142857142857" style="33" customWidth="1"/>
-    <col min="28" max="28" width="47.285714285714285" style="33" customWidth="1"/>
-    <col min="29" max="29" width="35.42857142857143" style="33" customWidth="1"/>
-    <col min="30" max="30" width="29.714285714285715" style="33" customWidth="1"/>
-    <col min="31" max="16384" width="15.285714285714286" style="33"/>
+    <col min="1" max="1" width="67.28571428571429" style="33" customWidth="1"/>
+    <col min="2" max="2" width="71.14285714285714" style="33" customWidth="1"/>
+    <col min="3" max="9" width="53.857142857142854" style="33" customWidth="1"/>
+    <col min="10" max="10" width="59.285714285714285" style="33" customWidth="1"/>
+    <col min="11" max="11" width="68" style="33" customWidth="1"/>
+    <col min="12" max="12" width="66.71428571428571" style="33" customWidth="1"/>
+    <col min="13" max="13" width="52.857142857142854" style="33" customWidth="1"/>
+    <col min="14" max="14" width="51.42857142857143" style="33" customWidth="1"/>
+    <col min="15" max="15" width="60" style="33" customWidth="1"/>
+    <col min="16" max="16" width="66" style="33" customWidth="1"/>
+    <col min="17" max="17" width="54.42857142857143" style="33" customWidth="1"/>
+    <col min="18" max="18" width="43.285714285714285" style="33" customWidth="1"/>
+    <col min="19" max="19" width="49.57142857142857" style="33" customWidth="1"/>
+    <col min="20" max="20" width="71.85714285714286" style="33" customWidth="1"/>
+    <col min="21" max="21" width="71.14285714285714" style="33" customWidth="1"/>
+    <col min="22" max="22" width="70.57142857142857" style="33" customWidth="1"/>
+    <col min="23" max="23" width="70.71428571428571" style="33" customWidth="1"/>
+    <col min="24" max="24" width="67.71428571428571" style="33" customWidth="1"/>
+    <col min="25" max="25" width="51" style="33" customWidth="1"/>
+    <col min="26" max="26" width="64.28571428571429" style="33" customWidth="1"/>
+    <col min="27" max="27" width="40.57142857142857" style="33" customWidth="1"/>
+    <col min="28" max="28" width="59" style="33" customWidth="1"/>
+    <col min="29" max="29" width="44.285714285714285" style="33" customWidth="1"/>
+    <col min="30" max="30" width="37" style="33" customWidth="1"/>
+    <col min="31" max="16384" width="19.142857142857142" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.05">
@@ -3496,33 +3692,33 @@
       <c r="AD16" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="3.7016" bottom="3.7016" header="3.5046999999999997" footer="3.5046999999999997"/>
+  <pageMargins left="0.7" right="0.7" top="4.8819" bottom="4.8819" header="4.685" footer="4.685"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75d71288-c06c-4cb0-abf3-95a5c20ca8b5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80ac50a5-2579-46e4-b75a-9cabcaf9af25}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="18.284285714285716" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="21.428571428571427" style="38" customWidth="1"/>
-    <col min="2" max="2" width="24.285714285714285" style="38" customWidth="1"/>
-    <col min="3" max="3" width="15.714285714285714" style="38" customWidth="1"/>
-    <col min="4" max="4" width="34" style="38" customWidth="1"/>
-    <col min="5" max="5" width="36.714285714285715" style="38" customWidth="1"/>
-    <col min="6" max="6" width="33.42857142857143" style="38" customWidth="1"/>
-    <col min="7" max="7" width="40.57142857142857" style="38" customWidth="1"/>
-    <col min="8" max="8" width="29.285714285714285" style="38" customWidth="1"/>
-    <col min="9" max="9" width="30.571428571428573" style="38" customWidth="1"/>
-    <col min="10" max="10" width="30.857142857142858" style="38" customWidth="1"/>
-    <col min="11" max="11" width="17.428571428571427" style="38" customWidth="1"/>
-    <col min="12" max="16384" width="14.571428571428571" style="38"/>
+    <col min="1" max="1" width="26.571428571428573" style="38" customWidth="1"/>
+    <col min="2" max="2" width="30.142857142857142" style="38" customWidth="1"/>
+    <col min="3" max="3" width="19.428571428571427" style="38" customWidth="1"/>
+    <col min="4" max="4" width="42.285714285714285" style="38" customWidth="1"/>
+    <col min="5" max="5" width="45.714285714285715" style="38" customWidth="1"/>
+    <col min="6" max="6" width="41.714285714285715" style="38" customWidth="1"/>
+    <col min="7" max="7" width="50.57142857142857" style="38" customWidth="1"/>
+    <col min="8" max="8" width="36.42857142857143" style="38" customWidth="1"/>
+    <col min="9" max="9" width="38" style="38" customWidth="1"/>
+    <col min="10" max="10" width="38.42857142857143" style="38" customWidth="1"/>
+    <col min="11" max="11" width="21.571428571428573" style="38" customWidth="1"/>
+    <col min="12" max="16384" width="18.285714285714285" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -3810,26 +4006,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336f71c6-9cab-4e65-8302-16fe22062728}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{de9c2a10-73e2-4b3c-822c-b4db7e4ac05f}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0" topLeftCell="C1">
+      <selection pane="topLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="18.284285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="14.142857142857142" style="38" customWidth="1"/>
-    <col min="2" max="2" width="30.428571428571427" style="38" customWidth="1"/>
-    <col min="3" max="3" width="28.857142857142858" style="38" customWidth="1"/>
-    <col min="4" max="4" width="17.428571428571427" style="38" customWidth="1"/>
-    <col min="5" max="5" width="38.142857142857146" style="38" customWidth="1"/>
-    <col min="6" max="6" width="32.857142857142854" style="38" customWidth="1"/>
-    <col min="7" max="7" width="34.142857142857146" style="38" customWidth="1"/>
-    <col min="8" max="8" width="33.285714285714285" style="38" customWidth="1"/>
-    <col min="9" max="9" width="33.142857142857146" style="38" customWidth="1"/>
-    <col min="10" max="10" width="33" style="38" customWidth="1"/>
-    <col min="11" max="16384" width="14.571428571428571" style="38"/>
+    <col min="1" max="1" width="17.428571428571427" style="38" customWidth="1"/>
+    <col min="2" max="2" width="37.857142857142854" style="38" customWidth="1"/>
+    <col min="3" max="3" width="35.857142857142854" style="38" customWidth="1"/>
+    <col min="4" max="4" width="21.571428571428573" style="38" customWidth="1"/>
+    <col min="5" max="5" width="47.57142857142857" style="38" customWidth="1"/>
+    <col min="6" max="6" width="41" style="38" customWidth="1"/>
+    <col min="7" max="7" width="42.42857142857143" style="38" customWidth="1"/>
+    <col min="8" max="8" width="41.42857142857143" style="38" customWidth="1"/>
+    <col min="9" max="9" width="41.285714285714285" style="38" customWidth="1"/>
+    <col min="10" max="10" width="41" style="38" customWidth="1"/>
+    <col min="11" max="16384" width="18.285714285714285" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">
@@ -4023,22 +4219,283 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403af5ea-a9f6-49a9-a546-a0a3dcc80686}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="12.8"/>
+  <cols>
+    <col min="1" max="1" width="29.571428571428573" style="47" customWidth="1"/>
+    <col min="2" max="2" width="26.714285714285715" style="47" customWidth="1"/>
+    <col min="3" max="5" width="33" style="47" customWidth="1"/>
+    <col min="6" max="6" width="41.857142857142854" style="47" customWidth="1"/>
+    <col min="7" max="7" width="34" style="47" customWidth="1"/>
+    <col min="8" max="8" width="32.142857142857146" style="47" customWidth="1"/>
+    <col min="9" max="16384" width="14.571428571428571" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.05">
+      <c r="A1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="12.8">
+      <c r="A2" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="45">
+        <v>377</v>
+      </c>
+      <c r="E2" s="49">
+        <v>124</v>
+      </c>
+      <c r="F2" s="45">
+        <v>7388</v>
+      </c>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+    </row>
+    <row r="3" spans="1:8" ht="12.8">
+      <c r="A3" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="45">
+        <v>377</v>
+      </c>
+      <c r="E3" s="49">
+        <v>124</v>
+      </c>
+      <c r="F3" s="45">
+        <v>7388</v>
+      </c>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.8">
+      <c r="A4" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:3" ht="12.8">
+      <c r="A5" s="46" t="s">
+        <v>321</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" s="45"/>
+    </row>
+    <row r="6" spans="1:3" ht="12.8">
+      <c r="A6" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="45"/>
+    </row>
+    <row r="7" spans="1:3" ht="12.8">
+      <c r="A7" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="45"/>
+    </row>
+    <row r="8" spans="1:3" ht="12.8">
+      <c r="A8" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7874" right="0.7874" top="1.0835000000000001" bottom="1.0835000000000001" header="0.9445000000000001" footer="0.9445000000000001"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88684db8-3251-44c4-b6af-dbe201bdf9af}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.574285714285713" defaultRowHeight="14.05"/>
+  <cols>
+    <col min="1" max="1" width="18.285714285714285" style="47" customWidth="1"/>
+    <col min="2" max="2" width="22.428571428571427" style="47" customWidth="1"/>
+    <col min="3" max="3" width="24" style="47" customWidth="1"/>
+    <col min="4" max="4" width="36.42857142857143" style="47" customWidth="1"/>
+    <col min="5" max="5" width="33.57142857142857" style="47" customWidth="1"/>
+    <col min="6" max="6" width="38.857142857142854" style="47" customWidth="1"/>
+    <col min="7" max="7" width="36.42857142857143" style="47" customWidth="1"/>
+    <col min="8" max="8" width="36.857142857142854" style="47" customWidth="1"/>
+    <col min="9" max="9" width="33.285714285714285" style="47" customWidth="1"/>
+    <col min="10" max="16384" width="14.571428571428571" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.05">
+      <c r="A1" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.05">
+      <c r="A2" s="53" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.05">
+      <c r="A3" s="54" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.05">
+      <c r="A4" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.05">
+      <c r="A5" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7874" right="0.7874" top="1.0835000000000001" bottom="1.0835000000000001" header="0.9445000000000001" footer="0.9445000000000001"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9f08c860-473f-424a-a6c4-53e8ee629f2d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0561ed4e-8f92-4892-8d89-51917e009b37}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="C1">
       <selection pane="topLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="52.857142857142854" style="3" customWidth="1"/>
-    <col min="2" max="2" width="64.14285714285714" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.857142857142854" style="3" customWidth="1"/>
-    <col min="4" max="4" width="78.42857142857143" style="3" customWidth="1"/>
-    <col min="5" max="5" width="98.42857142857143" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="66" style="3" customWidth="1"/>
+    <col min="2" max="2" width="80.14285714285714" style="3" customWidth="1"/>
+    <col min="3" max="3" width="77.28571428571429" style="3" customWidth="1"/>
+    <col min="4" max="4" width="97.85714285714286" style="3" customWidth="1"/>
+    <col min="5" max="5" width="123.14285714285714" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.05">
@@ -4093,25 +4550,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41391527-2827-4154-be93-f6c9d9b1329c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0767556d-9222-4bf4-8e7d-90f5676ff297}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="27" style="3"/>
-    <col min="2" max="2" width="94.71428571428571" style="3" customWidth="1"/>
-    <col min="3" max="3" width="84.14285714285714" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="33.857142857142854" style="3"/>
+    <col min="2" max="2" width="118.42857142857143" style="3" customWidth="1"/>
+    <col min="3" max="3" width="105.28571428571429" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.05">
@@ -4137,30 +4594,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30d8b873-4f3b-443d-8f12-45bfca2224d0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ef0d4c35-6b6c-4e81-a4ed-3e7fa5ae9d5f}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="71.85714285714286" style="3" customWidth="1"/>
-    <col min="2" max="2" width="108" style="3" customWidth="1"/>
-    <col min="3" max="3" width="83.42857142857143" style="3" customWidth="1"/>
-    <col min="4" max="4" width="73.71428571428571" style="3" customWidth="1"/>
-    <col min="5" max="5" width="63.714285714285715" style="3" customWidth="1"/>
-    <col min="6" max="6" width="70.57142857142857" style="3" customWidth="1"/>
-    <col min="7" max="8" width="63.714285714285715" style="3" customWidth="1"/>
-    <col min="9" max="9" width="59.714285714285715" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="89.85714285714286" style="3" customWidth="1"/>
+    <col min="2" max="2" width="135.28571428571428" style="3" customWidth="1"/>
+    <col min="3" max="3" width="104.14285714285714" style="3" customWidth="1"/>
+    <col min="4" max="4" width="92.14285714285714" style="3" customWidth="1"/>
+    <col min="5" max="5" width="79.57142857142857" style="3" customWidth="1"/>
+    <col min="6" max="6" width="88.14285714285714" style="3" customWidth="1"/>
+    <col min="7" max="8" width="79.57142857142857" style="3" customWidth="1"/>
+    <col min="9" max="9" width="74.57142857142857" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.05">
@@ -4309,30 +4766,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5a994e50-2ed2-4850-98c1-54f0265d9ced}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{c5d7fc7a-e7b2-4b2d-97f5-523da17a4ccf}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="99.57142857142857" style="3" customWidth="1"/>
-    <col min="2" max="2" width="139.28571428571428" style="3" customWidth="1"/>
-    <col min="3" max="3" width="75.28571428571429" style="3" customWidth="1"/>
-    <col min="4" max="4" width="97.71428571428571" style="3" customWidth="1"/>
-    <col min="5" max="5" width="92.57142857142857" style="3" customWidth="1"/>
-    <col min="6" max="6" width="71.85714285714286" style="3" customWidth="1"/>
-    <col min="7" max="7" width="82.85714285714286" style="3" customWidth="1"/>
-    <col min="8" max="8" width="110.14285714285714" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="124.57142857142857" style="3" customWidth="1"/>
+    <col min="2" max="2" width="174.42857142857142" style="3" customWidth="1"/>
+    <col min="3" max="3" width="94.14285714285714" style="3" customWidth="1"/>
+    <col min="4" max="4" width="122.28571428571429" style="3" customWidth="1"/>
+    <col min="5" max="5" width="115.71428571428571" style="3" customWidth="1"/>
+    <col min="6" max="6" width="89.85714285714286" style="3" customWidth="1"/>
+    <col min="7" max="7" width="103.42857142857143" style="3" customWidth="1"/>
+    <col min="8" max="8" width="137.85714285714286" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.05">
@@ -4518,31 +4975,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d6dac21d-1c4b-443f-ae7a-40cb8690d10a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{fd9905d2-6ef5-4500-902a-a3a9a5015d53}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.004285714285714" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="33.854285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="65.42857142857143" style="3" customWidth="1"/>
-    <col min="2" max="2" width="84.57142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="81.71428571428571" style="3" customWidth="1"/>
-    <col min="4" max="4" width="79.57142857142857" style="3" customWidth="1"/>
-    <col min="5" max="5" width="50" style="3" customWidth="1"/>
-    <col min="6" max="7" width="27" style="3"/>
-    <col min="8" max="9" width="69.14285714285714" style="3" customWidth="1"/>
-    <col min="10" max="10" width="45.285714285714285" style="3" customWidth="1"/>
-    <col min="11" max="11" width="55.857142857142854" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="27" style="3"/>
+    <col min="1" max="1" width="81.71428571428571" style="3" customWidth="1"/>
+    <col min="2" max="2" width="105.71428571428571" style="3" customWidth="1"/>
+    <col min="3" max="3" width="102.28571428571429" style="3" customWidth="1"/>
+    <col min="4" max="4" width="99.57142857142857" style="3" customWidth="1"/>
+    <col min="5" max="5" width="62.42857142857143" style="3" customWidth="1"/>
+    <col min="6" max="7" width="33.857142857142854" style="3"/>
+    <col min="8" max="9" width="86.42857142857143" style="3" customWidth="1"/>
+    <col min="10" max="10" width="56.42857142857143" style="3" customWidth="1"/>
+    <col min="11" max="11" width="69.71428571428571" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="33.857142857142854" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.05">
@@ -4706,39 +5163,39 @@
       <c r="J6" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69342407-d2b7-4fec-8e82-ca1e0d471fb8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74453d6e-f3b7-4b0d-b6a9-831f3eda934d}">
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="S1">
       <selection pane="topLeft" activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.854285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="33.714285714285715" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="52.857142857142854" style="13" customWidth="1"/>
-    <col min="2" max="2" width="78" style="13" customWidth="1"/>
-    <col min="3" max="3" width="86.28571428571429" style="13" customWidth="1"/>
-    <col min="4" max="4" width="57.285714285714285" style="13" customWidth="1"/>
-    <col min="5" max="6" width="85" style="13" customWidth="1"/>
-    <col min="7" max="7" width="70.57142857142857" style="13" customWidth="1"/>
-    <col min="8" max="9" width="63.42857142857143" style="13" customWidth="1"/>
-    <col min="10" max="10" width="78" style="13" customWidth="1"/>
-    <col min="11" max="11" width="67.85714285714286" style="13" customWidth="1"/>
-    <col min="12" max="12" width="60.285714285714285" style="13" customWidth="1"/>
-    <col min="13" max="13" width="59" style="13" customWidth="1"/>
-    <col min="14" max="14" width="52.857142857142854" style="13" customWidth="1"/>
-    <col min="15" max="15" width="25" style="13" customWidth="1"/>
-    <col min="16" max="20" width="57.57142857142857" style="13" customWidth="1"/>
-    <col min="21" max="22" width="40.57142857142857" style="13" customWidth="1"/>
-    <col min="23" max="24" width="66.28571428571429" style="13" customWidth="1"/>
-    <col min="25" max="25" width="47.57142857142857" style="13" customWidth="1"/>
-    <col min="26" max="16384" width="26.857142857142858" style="13"/>
+    <col min="1" max="1" width="66" style="13" customWidth="1"/>
+    <col min="2" max="2" width="97.42857142857143" style="13" customWidth="1"/>
+    <col min="3" max="3" width="108" style="13" customWidth="1"/>
+    <col min="4" max="4" width="71.57142857142857" style="13" customWidth="1"/>
+    <col min="5" max="6" width="106.14285714285714" style="13" customWidth="1"/>
+    <col min="7" max="7" width="88.14285714285714" style="13" customWidth="1"/>
+    <col min="8" max="9" width="79.14285714285714" style="13" customWidth="1"/>
+    <col min="10" max="10" width="97.42857142857143" style="13" customWidth="1"/>
+    <col min="11" max="11" width="84.71428571428571" style="13" customWidth="1"/>
+    <col min="12" max="12" width="75.28571428571429" style="13" customWidth="1"/>
+    <col min="13" max="13" width="73.71428571428571" style="13" customWidth="1"/>
+    <col min="14" max="14" width="66" style="13" customWidth="1"/>
+    <col min="15" max="15" width="31.142857142857142" style="13" customWidth="1"/>
+    <col min="16" max="20" width="71.85714285714286" style="13" customWidth="1"/>
+    <col min="21" max="22" width="50.57142857142857" style="13" customWidth="1"/>
+    <col min="23" max="24" width="82.85714285714286" style="13" customWidth="1"/>
+    <col min="25" max="25" width="59.285714285714285" style="13" customWidth="1"/>
+    <col min="26" max="16384" width="33.714285714285715" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.05">
@@ -5478,35 +5935,35 @@
       <c r="Y12" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4c1baa5d-7fb4-482f-8342-d55018f6955b}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61066efc-24ab-416c-9ae2-f323dcb3b5f7}">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.854285714285716" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="33.714285714285715" defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="48.714285714285715" style="13" customWidth="1"/>
-    <col min="2" max="2" width="83.42857142857143" style="13" customWidth="1"/>
-    <col min="3" max="3" width="19.857142857142858" style="13" customWidth="1"/>
-    <col min="4" max="5" width="73.14285714285714" style="13" customWidth="1"/>
-    <col min="6" max="6" width="64.14285714285714" style="13" customWidth="1"/>
-    <col min="7" max="7" width="77.85714285714286" style="13" customWidth="1"/>
-    <col min="8" max="8" width="75.28571428571429" style="13" customWidth="1"/>
-    <col min="9" max="9" width="53.42857142857143" style="13" customWidth="1"/>
-    <col min="10" max="10" width="66" style="13" customWidth="1"/>
-    <col min="11" max="11" width="64" style="13" customWidth="1"/>
-    <col min="12" max="12" width="52.42857142857143" style="13" customWidth="1"/>
-    <col min="13" max="13" width="34.42857142857143" style="13" customWidth="1"/>
-    <col min="14" max="14" width="42.57142857142857" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="26.857142857142858" style="13"/>
+    <col min="1" max="1" width="60.857142857142854" style="13" customWidth="1"/>
+    <col min="2" max="2" width="104.14285714285714" style="13" customWidth="1"/>
+    <col min="3" max="3" width="24.571428571428573" style="13" customWidth="1"/>
+    <col min="4" max="5" width="91.42857142857143" style="13" customWidth="1"/>
+    <col min="6" max="6" width="80.14285714285714" style="13" customWidth="1"/>
+    <col min="7" max="7" width="97.28571428571429" style="13" customWidth="1"/>
+    <col min="8" max="8" width="94.14285714285714" style="13" customWidth="1"/>
+    <col min="9" max="9" width="66.71428571428571" style="13" customWidth="1"/>
+    <col min="10" max="10" width="82.42857142857143" style="13" customWidth="1"/>
+    <col min="11" max="11" width="80" style="13" customWidth="1"/>
+    <col min="12" max="12" width="65.42857142857143" style="13" customWidth="1"/>
+    <col min="13" max="13" width="42.857142857142854" style="13" customWidth="1"/>
+    <col min="14" max="14" width="53.142857142857146" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="33.714285714285715" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.05">
@@ -6346,30 +6803,30 @@
       <c r="N23" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="6.6528" bottom="6.6528" header="6.4559" footer="6.4559"/>
+  <pageMargins left="0.7" right="0.7" top="7.8335" bottom="7.8335" header="7.6366" footer="7.6366"/>
   <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1beb3ac7-bc64-4d3b-8d44-2c890b47a65a}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4f4b1d0d-f6d4-412d-8f1f-fd773ee81e9a}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection pane="topLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.144285714285715" defaultRowHeight="14.05"/>
+  <sheetFormatPr defaultColWidth="30.284285714285716" defaultRowHeight="14.05"/>
   <cols>
-    <col min="1" max="1" width="25.285714285714285" style="26" customWidth="1"/>
-    <col min="2" max="2" width="128.57142857142858" style="26" customWidth="1"/>
-    <col min="3" max="3" width="97.28571428571429" style="26" customWidth="1"/>
-    <col min="4" max="4" width="19.428571428571427" style="26" customWidth="1"/>
-    <col min="5" max="7" width="112.42857142857143" style="26" customWidth="1"/>
-    <col min="8" max="8" width="75.28571428571429" style="26" customWidth="1"/>
-    <col min="9" max="9" width="74.57142857142857" style="26" customWidth="1"/>
-    <col min="10" max="10" width="71.85714285714286" style="26" customWidth="1"/>
-    <col min="11" max="16384" width="24.142857142857142" style="13"/>
+    <col min="1" max="1" width="31.428571428571427" style="26" customWidth="1"/>
+    <col min="2" max="2" width="161" style="26" customWidth="1"/>
+    <col min="3" max="3" width="121.57142857142857" style="26" customWidth="1"/>
+    <col min="4" max="4" width="24" style="26" customWidth="1"/>
+    <col min="5" max="7" width="140.71428571428572" style="26" customWidth="1"/>
+    <col min="8" max="8" width="94.14285714285714" style="26" customWidth="1"/>
+    <col min="9" max="9" width="93.14285714285714" style="26" customWidth="1"/>
+    <col min="10" max="10" width="89.85714285714286" style="26" customWidth="1"/>
+    <col min="11" max="16384" width="30.285714285714285" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.05">

</xml_diff>

<commit_message>
Commit on 02 06 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMTestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="387">
   <si>
     <t>Stage</t>
   </si>
@@ -1215,34 +1215,40 @@
     <t>Debit Amount Two</t>
   </si>
   <si>
-    <t>7735</t>
-  </si>
-  <si>
-    <t>7736</t>
-  </si>
-  <si>
-    <t>7737</t>
-  </si>
-  <si>
-    <t>7738</t>
-  </si>
-  <si>
-    <t>7739</t>
-  </si>
-  <si>
-    <t>7749</t>
-  </si>
-  <si>
-    <t>7750</t>
-  </si>
-  <si>
-    <t>7752</t>
-  </si>
-  <si>
-    <t>7753</t>
-  </si>
-  <si>
-    <t>7754</t>
+    <t>7755</t>
+  </si>
+  <si>
+    <t>7756</t>
+  </si>
+  <si>
+    <t>7757</t>
+  </si>
+  <si>
+    <t>7758</t>
+  </si>
+  <si>
+    <t>7759</t>
+  </si>
+  <si>
+    <t>586</t>
+  </si>
+  <si>
+    <t>292124</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>7801</t>
+  </si>
+  <si>
+    <t>7809</t>
+  </si>
+  <si>
+    <t>7811</t>
+  </si>
+  <si>
+    <t>7813</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1561,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1640,7 +1646,6 @@
     <xf numFmtId="49" fontId="1" fillId="13" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="16" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="13" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="19" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
@@ -4513,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75"/>
@@ -4964,7 +4969,9 @@
       <c r="C9" s="51" t="s">
         <v>324</v>
       </c>
-      <c r="D9" s="76"/>
+      <c r="D9" s="76" t="s">
+        <v>384</v>
+      </c>
       <c r="E9" s="72">
         <v>377</v>
       </c>
@@ -4972,17 +4979,17 @@
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
-      <c r="J9" s="74">
-        <v>1</v>
-      </c>
-      <c r="K9" s="74">
-        <v>840</v>
-      </c>
-      <c r="L9" s="74">
-        <v>96148</v>
-      </c>
-      <c r="M9" s="74">
-        <v>993598</v>
+      <c r="J9" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="K9" s="74" t="s">
+        <v>380</v>
+      </c>
+      <c r="L9" s="74" t="s">
+        <v>381</v>
+      </c>
+      <c r="M9" s="74" t="s">
+        <v>382</v>
       </c>
       <c r="N9" s="74">
         <v>0</v>
@@ -5027,16 +5034,16 @@
       <c r="J10" s="74" t="s">
         <v>367</v>
       </c>
-      <c r="K10" s="79" t="s">
+      <c r="K10" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="79" t="s">
+      <c r="L10" s="78" t="s">
         <v>368</v>
       </c>
-      <c r="M10" s="79" t="s">
+      <c r="M10" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="N10" s="79" t="s">
+      <c r="N10" s="78" t="s">
         <v>136</v>
       </c>
       <c r="O10" s="74">
@@ -5046,17 +5053,17 @@
         <v>1000</v>
       </c>
       <c r="Q10" s="77"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="78"/>
-      <c r="T10" s="78"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="78"/>
-      <c r="W10" s="78"/>
-      <c r="X10" s="78"/>
-      <c r="Y10" s="78"/>
-      <c r="Z10" s="78"/>
-      <c r="AA10" s="78"/>
-      <c r="AB10" s="78"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="70"/>
+      <c r="W10" s="70"/>
+      <c r="X10" s="70"/>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="70"/>
+      <c r="AB10" s="70"/>
     </row>
     <row r="11" spans="1:28">
       <c r="A11" s="69" t="s">
@@ -5069,7 +5076,7 @@
         <v>324</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E11" s="72">
         <v>377</v>
@@ -5100,17 +5107,17 @@
         <v>1000</v>
       </c>
       <c r="Q11" s="77"/>
-      <c r="R11" s="78"/>
-      <c r="S11" s="78"/>
-      <c r="T11" s="78"/>
-      <c r="U11" s="78"/>
-      <c r="V11" s="78"/>
-      <c r="W11" s="78"/>
-      <c r="X11" s="78"/>
-      <c r="Y11" s="78"/>
-      <c r="Z11" s="78"/>
-      <c r="AA11" s="78"/>
-      <c r="AB11" s="78"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="70"/>
+      <c r="W11" s="70"/>
+      <c r="X11" s="70"/>
+      <c r="Y11" s="70"/>
+      <c r="Z11" s="70"/>
+      <c r="AA11" s="70"/>
+      <c r="AB11" s="70"/>
     </row>
     <row r="12" spans="1:28">
       <c r="A12" s="69" t="s">
@@ -5123,7 +5130,7 @@
         <v>324</v>
       </c>
       <c r="D12" s="76" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E12" s="72" t="s">
         <v>134</v>
@@ -5138,10 +5145,10 @@
       <c r="K12" s="74">
         <v>840</v>
       </c>
-      <c r="L12" s="79" t="s">
+      <c r="L12" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="M12" s="79" t="s">
+      <c r="M12" s="78" t="s">
         <v>82</v>
       </c>
       <c r="N12" s="74">
@@ -5156,7 +5163,7 @@
       <c r="Q12" s="77">
         <v>2</v>
       </c>
-      <c r="R12" s="79">
+      <c r="R12" s="78">
         <v>840</v>
       </c>
       <c r="S12" s="74" t="s">
@@ -5165,16 +5172,16 @@
       <c r="T12" s="74">
         <v>0</v>
       </c>
-      <c r="U12" s="79">
+      <c r="U12" s="78">
         <v>0</v>
       </c>
-      <c r="V12" s="78"/>
-      <c r="W12" s="78"/>
-      <c r="X12" s="78"/>
-      <c r="Y12" s="78"/>
-      <c r="Z12" s="78"/>
-      <c r="AA12" s="78"/>
-      <c r="AB12" s="78"/>
+      <c r="V12" s="70"/>
+      <c r="W12" s="70"/>
+      <c r="X12" s="70"/>
+      <c r="Y12" s="70"/>
+      <c r="Z12" s="70"/>
+      <c r="AA12" s="70"/>
+      <c r="AB12" s="70"/>
     </row>
     <row r="13" spans="1:28">
       <c r="A13" s="69" t="s">
@@ -5187,7 +5194,7 @@
         <v>324</v>
       </c>
       <c r="D13" s="76" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E13" s="72" t="s">
         <v>367</v>
@@ -5217,40 +5224,40 @@
       <c r="P13" s="75">
         <v>1000</v>
       </c>
-      <c r="Q13" s="79" t="s">
+      <c r="Q13" s="78" t="s">
         <v>367</v>
       </c>
-      <c r="R13" s="79" t="s">
+      <c r="R13" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="S13" s="79" t="s">
+      <c r="S13" s="78" t="s">
         <v>368</v>
       </c>
-      <c r="T13" s="79" t="s">
+      <c r="T13" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="U13" s="79" t="s">
+      <c r="U13" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="V13" s="79" t="s">
+      <c r="V13" s="78" t="s">
         <v>369</v>
       </c>
-      <c r="W13" s="79" t="s">
+      <c r="W13" s="78" t="s">
         <v>371</v>
       </c>
-      <c r="X13" s="79" t="s">
+      <c r="X13" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="Y13" s="79" t="s">
+      <c r="Y13" s="78" t="s">
         <v>372</v>
       </c>
-      <c r="Z13" s="79" t="s">
+      <c r="Z13" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="AA13" s="79" t="s">
+      <c r="AA13" s="78" t="s">
         <v>373</v>
       </c>
-      <c r="AB13" s="79" t="s">
+      <c r="AB13" s="78" t="s">
         <v>369</v>
       </c>
     </row>
@@ -5265,7 +5272,7 @@
         <v>324</v>
       </c>
       <c r="D14" s="76" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E14" s="72">
         <v>377</v>
@@ -5296,17 +5303,17 @@
         <v>1000</v>
       </c>
       <c r="Q14" s="77"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="78"/>
-      <c r="T14" s="78"/>
-      <c r="U14" s="78"/>
-      <c r="V14" s="78"/>
-      <c r="W14" s="78"/>
-      <c r="X14" s="78"/>
-      <c r="Y14" s="78"/>
-      <c r="Z14" s="78"/>
-      <c r="AA14" s="78"/>
-      <c r="AB14" s="78"/>
+      <c r="R14" s="70"/>
+      <c r="S14" s="70"/>
+      <c r="T14" s="70"/>
+      <c r="U14" s="70"/>
+      <c r="V14" s="70"/>
+      <c r="W14" s="70"/>
+      <c r="X14" s="70"/>
+      <c r="Y14" s="70"/>
+      <c r="Z14" s="70"/>
+      <c r="AA14" s="70"/>
+      <c r="AB14" s="70"/>
     </row>
     <row r="15" spans="1:28">
       <c r="A15" s="69" t="s">
@@ -5319,7 +5326,7 @@
         <v>324</v>
       </c>
       <c r="D15" s="76" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E15" s="72" t="s">
         <v>134</v>
@@ -5334,10 +5341,10 @@
       <c r="K15" s="74">
         <v>840</v>
       </c>
-      <c r="L15" s="79">
+      <c r="L15" s="78">
         <v>96145</v>
       </c>
-      <c r="M15" s="79">
+      <c r="M15" s="78">
         <v>993579</v>
       </c>
       <c r="N15" s="74">
@@ -5349,10 +5356,10 @@
       <c r="P15" s="75">
         <v>100</v>
       </c>
-      <c r="Q15" s="80">
+      <c r="Q15" s="79">
         <v>2</v>
       </c>
-      <c r="R15" s="79">
+      <c r="R15" s="78">
         <v>840</v>
       </c>
       <c r="S15" s="74">
@@ -5361,16 +5368,16 @@
       <c r="T15" s="74">
         <v>0</v>
       </c>
-      <c r="U15" s="79">
+      <c r="U15" s="78">
         <v>0</v>
       </c>
-      <c r="V15" s="78"/>
-      <c r="W15" s="78"/>
-      <c r="X15" s="78"/>
-      <c r="Y15" s="78"/>
-      <c r="Z15" s="78"/>
-      <c r="AA15" s="78"/>
-      <c r="AB15" s="78"/>
+      <c r="V15" s="70"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="70"/>
+      <c r="Y15" s="70"/>
+      <c r="Z15" s="70"/>
+      <c r="AA15" s="70"/>
+      <c r="AB15" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.0835000000000001" bottom="1.0835000000000001" header="0.94450000000000012" footer="0.94450000000000012"/>
@@ -5387,14 +5394,14 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="49" width="28.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="49" width="34.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="49" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="49" width="14.80078125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="49" width="56.42578125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="49" width="52.42578125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="49" width="60.28515625" collapsed="true"/>
@@ -5636,7 +5643,7 @@
         <v>360</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>226</v>
+        <v>95</v>
       </c>
       <c r="D13" s="50" t="s">
         <v>337</v>
@@ -5655,7 +5662,7 @@
         <v>338</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>226</v>
+        <v>95</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
@@ -5717,7 +5724,7 @@
         <v>347</v>
       </c>
       <c r="F17" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G17" s="50"/>
       <c r="H17" s="50"/>
@@ -5731,7 +5738,7 @@
         <v>342</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
@@ -5748,7 +5755,7 @@
         <v>348</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
@@ -5765,7 +5772,7 @@
         <v>346</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>

</xml_diff>